<commit_message>
Codes update (apr 26 deployment)
</commit_message>
<xml_diff>
--- a/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
+++ b/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/ske5_cdc_gov/Documents/+My_Documents/Shilpa/CPT/downloads/New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B11A90B-ED5F-40BC-A65F-D1C10E5748AA}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D7EB78-1A57-44AD-8EF2-D9D212F8023D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WEB cvx list" sheetId="47" r:id="rId1"/>
+    <sheet name="WEB cvx list" sheetId="48" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" localSheetId="0" hidden="1">'WEB cvx list'!$A$1:$H$239</definedName>
+    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" localSheetId="0" hidden="1">'WEB cvx list'!$A$1:$H$247</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -24,14 +24,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{ED7E5AE7-4B40-4367-A4C0-1D89997A1DFE}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes11111111111111111111111111" type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="1" xr16:uid="{ED0B1E6E-28B3-4E4A-ABD9-3F47F544470F}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes111111111111111111111111111" type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;User ID=insidenipdbo;Initial Catalog=NIP_INSIDENIP;Data Source=DSDV-INFC-1601\qsrv1;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=D314248;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;NIP_INSIDENIP&quot;.&quot;dbo&quot;.&quot;tblCVXCodes&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="826">
   <si>
     <t>CVX Code</t>
   </si>
@@ -2428,6 +2428,87 @@
   </si>
   <si>
     <t>FDA EUA 03/29/2022, Moderna booster dose 2.5mL vial presentation only</t>
+  </si>
+  <si>
+    <t>512</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 VLP Non-US Vaccine (Medicago, Covifenz)</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 Virus Like Particle (VLP) Non-US Vaccine Product (Medicago, Covifenz)</t>
+  </si>
+  <si>
+    <t>Pandemic Non-US Vaccine not Authorized by WHO - ACIP does recognize towards immunity in US</t>
+  </si>
+  <si>
+    <t>513</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 PS Non-US Vaccine (Anhui Zhifei Longcom, Zifivax)</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 Protein Subunit Non-US Vaccine Product (Anhui Zhifei Longcom, Zifivax)</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 DNA Non-US Vaccine (Zydus Cadila, ZyCoV-D)</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 DNA Non-US Vaccine Product (Zydus Cadila, ZyCoV-D)</t>
+  </si>
+  <si>
+    <t>515</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 PS Non-US Vaccine (Medigen, MVC-COV1901)</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 Protein Subunit Non-US Vaccine Product (Medigen, MVC-COV1901)</t>
+  </si>
+  <si>
+    <t>516</t>
+  </si>
+  <si>
+    <t>COV-2 COVID-19 Inactivated Non-US Vaccine Product (Minhai Biotechnology Co, KCONVAC)</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 Inactivated Non-US Vaccine Product (Minhai Biotechnology Co, KCONVAC)</t>
+  </si>
+  <si>
+    <t>517</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 PS Non-US Vaccine (Biological E Limited, Corbevax)</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 COVID-19 Protein Subunit Non-US Vaccine Product (Biological E Limited, Corbevax)</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>COVID-19, mRNA, LNP-S, PF, pediatric 50 mcg/0.5 mL dose</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 (COVID-19) vaccine, mRNA, spike protein, LNP, preservative free, pediatric 50 mcg/0.5 mL dose</t>
+  </si>
+  <si>
+    <t>Pre-EUA Moderna Pediatric 6yr to&lt;12 yr vaccine 2.5 mL vial, 50 mcg/0.5 mL dose</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>COVID-19, mRNA, LNP-S, PF, pediatric 25 mcg/0.25 mL dose</t>
+  </si>
+  <si>
+    <t>SARS-COV-2 (COVID-19) vaccine, mRNA, spike protein, LNP, preservative free, pediatric 25 mcg/0.25 mL dose</t>
+  </si>
+  <si>
+    <t>Pre-EUA Moderna Pediatric 6mo to&lt;6yr 2.5 mL vial, 25 mcg/0.25 mL dose</t>
   </si>
 </sst>
 </file>
@@ -2435,7 +2516,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -2475,7 +2556,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2491,7 +2572,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes_1" connectionId="1" xr16:uid="{EF101FE4-4086-4396-9F8F-191A84734629}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes" connectionId="1" xr16:uid="{9F851C33-44E3-421E-8029-DB537F28EAFA}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="11">
     <queryTableFields count="8">
       <queryTableField id="2" name="cvx_code" tableColumnId="2"/>
@@ -2511,16 +2592,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C59044EB-852A-4634-A34B-F161A521B6BD}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" ref="A1:H239" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BCA8BF2C-20C2-4C01-A9A1-E26E0C7CD2B0}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" ref="A1:H247" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{62823254-6479-441F-90FD-DECD59D91DC0}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{D31DA72F-629A-4EE5-8B18-C52AD196FE64}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{934F6B8F-B58D-4393-A359-56FE39EA6C32}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{F2DE8279-FAB0-4449-9BA5-1A4C10A90084}" uniqueName="5" name="Note" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{059A9EBB-0C55-41C7-BF8B-F8C568758BBE}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
-    <tableColumn id="1" xr3:uid="{06C55A2D-D90A-4B77-BBDC-B12220EF17D2}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
-    <tableColumn id="8" xr3:uid="{7B2E4500-FEE2-4CE4-9AE9-5CF2A1C7E1D9}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{98FA754C-3927-49E1-9DA9-87981018FFE1}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{F2654376-AF8E-4C2A-BDA2-4C8E6A9F52CF}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{DF8A440B-53A7-4B06-97E4-FCB436AE01B8}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{4A00DA9F-1F34-45A9-A9F1-36CB98A0A39F}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{1105948F-93AC-4B5B-8B9A-CE8C8D74B959}" uniqueName="5" name="Note" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{14D5DC58-669F-414B-B5A6-D56A7FBBEE1F}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{6241FCBF-E936-468C-81AB-A0363389F43B}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
+    <tableColumn id="8" xr3:uid="{B9F4AD64-E9E6-429F-8FBB-BFDFA7DA7819}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{BFAF6871-50AB-4D2E-8406-219495F631BB}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2846,24 +2927,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8946C10C-C798-47F5-907C-8094165B04CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C90FE9E-F67E-49C9-9B0E-08DFB6E83501}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H239"/>
+  <dimension ref="A1:H247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="H233" sqref="H233"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
     <col min="3" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8974,7 +9055,7 @@
         <v>615</v>
       </c>
       <c r="H235" s="1">
-        <v>44623</v>
+        <v>44636</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
@@ -9081,9 +9162,217 @@
         <v>44630</v>
       </c>
     </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>799</v>
+      </c>
+      <c r="B240" t="s">
+        <v>800</v>
+      </c>
+      <c r="C240" t="s">
+        <v>801</v>
+      </c>
+      <c r="D240" t="s">
+        <v>802</v>
+      </c>
+      <c r="E240" t="s">
+        <v>50</v>
+      </c>
+      <c r="F240">
+        <v>262</v>
+      </c>
+      <c r="G240" t="s">
+        <v>615</v>
+      </c>
+      <c r="H240" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>803</v>
+      </c>
+      <c r="B241" t="s">
+        <v>804</v>
+      </c>
+      <c r="C241" t="s">
+        <v>805</v>
+      </c>
+      <c r="D241" t="s">
+        <v>710</v>
+      </c>
+      <c r="E241" t="s">
+        <v>50</v>
+      </c>
+      <c r="F241">
+        <v>263</v>
+      </c>
+      <c r="G241" t="s">
+        <v>615</v>
+      </c>
+      <c r="H241" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>806</v>
+      </c>
+      <c r="B242" t="s">
+        <v>807</v>
+      </c>
+      <c r="C242" t="s">
+        <v>808</v>
+      </c>
+      <c r="D242" t="s">
+        <v>710</v>
+      </c>
+      <c r="E242" t="s">
+        <v>50</v>
+      </c>
+      <c r="F242">
+        <v>264</v>
+      </c>
+      <c r="G242" t="s">
+        <v>615</v>
+      </c>
+      <c r="H242" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>809</v>
+      </c>
+      <c r="B243" t="s">
+        <v>810</v>
+      </c>
+      <c r="C243" t="s">
+        <v>811</v>
+      </c>
+      <c r="D243" t="s">
+        <v>710</v>
+      </c>
+      <c r="E243" t="s">
+        <v>50</v>
+      </c>
+      <c r="F243">
+        <v>265</v>
+      </c>
+      <c r="G243" t="s">
+        <v>615</v>
+      </c>
+      <c r="H243" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>812</v>
+      </c>
+      <c r="B244" t="s">
+        <v>813</v>
+      </c>
+      <c r="C244" t="s">
+        <v>814</v>
+      </c>
+      <c r="D244" t="s">
+        <v>710</v>
+      </c>
+      <c r="E244" t="s">
+        <v>50</v>
+      </c>
+      <c r="F244">
+        <v>266</v>
+      </c>
+      <c r="G244" t="s">
+        <v>615</v>
+      </c>
+      <c r="H244" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>815</v>
+      </c>
+      <c r="B245" t="s">
+        <v>816</v>
+      </c>
+      <c r="C245" t="s">
+        <v>817</v>
+      </c>
+      <c r="D245" t="s">
+        <v>710</v>
+      </c>
+      <c r="E245" t="s">
+        <v>50</v>
+      </c>
+      <c r="F245">
+        <v>267</v>
+      </c>
+      <c r="G245" t="s">
+        <v>615</v>
+      </c>
+      <c r="H245" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>818</v>
+      </c>
+      <c r="B246" t="s">
+        <v>819</v>
+      </c>
+      <c r="C246" t="s">
+        <v>820</v>
+      </c>
+      <c r="D246" t="s">
+        <v>821</v>
+      </c>
+      <c r="E246" t="s">
+        <v>23</v>
+      </c>
+      <c r="F246">
+        <v>268</v>
+      </c>
+      <c r="G246" t="s">
+        <v>615</v>
+      </c>
+      <c r="H246" s="1">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>822</v>
+      </c>
+      <c r="B247" t="s">
+        <v>823</v>
+      </c>
+      <c r="C247" t="s">
+        <v>824</v>
+      </c>
+      <c r="D247" t="s">
+        <v>825</v>
+      </c>
+      <c r="E247" t="s">
+        <v>23</v>
+      </c>
+      <c r="F247">
+        <v>269</v>
+      </c>
+      <c r="G247" t="s">
+        <v>615</v>
+      </c>
+      <c r="H247" s="1">
+        <v>44663</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="20" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="19" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Send registration notification to list of admins, update codes
</commit_message>
<xml_diff>
--- a/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
+++ b/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/ske5_cdc_gov/Documents/+My_Documents/Shilpa/CPT/downloads/New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="494" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19085CB5-7C95-4410-BC0B-51D5F4892C2A}"/>
+  <xr:revisionPtr revIDLastSave="541" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{279E5923-5567-4697-A4F3-8BA19322578E}"/>
   <bookViews>
-    <workbookView xWindow="1788" yWindow="792" windowWidth="21252" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="444" windowWidth="21252" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_cvx" sheetId="64" r:id="rId1"/>
+    <sheet name="Web_cvx" sheetId="66" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" localSheetId="0" hidden="1">Web_cvx!$A$1:$H$268</definedName>
+    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" localSheetId="0" hidden="1">Web_cvx!$A$1:$H$271</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -24,14 +24,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{6794FB14-FE8E-4BC3-845A-C22290BC57B2}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes1111111111111111111111111111111111111111111" type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{AF79F891-6952-46A0-889A-A4420FC1CBF5}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes111111111111111111111111111111111111111111111" type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;User ID=insidenipdbo;Initial Catalog=NIP_INSIDENIP;Data Source=DSDV-INFC-1601\qsrv1;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=D314248;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;NIP_INSIDENIP&quot;.&quot;dbo&quot;.&quot;tblCVXCodes&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="916">
   <si>
     <t>CVX Code</t>
   </si>
@@ -2280,9 +2280,6 @@
     <t>Non-US vaccine</t>
   </si>
   <si>
-    <t>FDA EUA 02/27/2021, 1-dose vaccine. Used to record Janssen/J&amp;J vaccines administered in the US and in non-US locations</t>
-  </si>
-  <si>
     <t>COVID-19, subunit, rS-nanoparticle+Matrix-M1 Adjuvant, PF, 0.5 mL</t>
   </si>
   <si>
@@ -2421,9 +2418,6 @@
     <t>Applies to tetravalent product (e.g. DENGVAXIA)</t>
   </si>
   <si>
-    <t>Temporarily inactivated -  Use CVX code 221 for EUA Moderna Pediatric 6yr to&lt;12 yr vaccine 2.5 mL vial, 50 mcg/0.5 mL dose</t>
-  </si>
-  <si>
     <t>229</t>
   </si>
   <si>
@@ -2442,27 +2436,6 @@
     <t>300</t>
   </si>
   <si>
-    <t>FDA EUA and BLA (18+ yrs), Moderna adult primary series and IC dose. EUA 8/31/2022 rescinded monovalent booster dose. Used to record Moderna vaccines administered in the US and in non-US locations (includes tradename Spikevax)</t>
-  </si>
-  <si>
-    <t>FDA EUA (12+ yrs) and BLA (16+ yrs), Pfizer adult primary series and IC dose original formulation. EUA 8/31/2022 rescinded monovalent booster dose. Used to record Pfizer vaccines administered in the US and in non-US locations (includes tradename Comirnaty)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FDA EUA (6 mo through 4 yrs), Pfizer tris-sucrose pediatric primary series </t>
-  </si>
-  <si>
-    <t>FDA EUA (12+ yrs) and BLA (16+ yrs), Pfizer adult primary series and IC dose tris-sucrose formulation. EUA 8/31/2022 rescinded monovalent booster dose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FDA EUA (5 yrs through 11 yrs), Pfizer tris-sucrose pediatric primary series, IC, and booster </t>
-  </si>
-  <si>
-    <t>FDA EUA Moderna, EUA 8/31/2022 rescinded use of this product for adult monovalent booster dose.  Vaccine now only authorized for 6 yrs through 11 primary series and IC doses</t>
-  </si>
-  <si>
-    <t>FDA EUA Authorized (6 mo through 5 yrs), Moderna pediatric primary series and IC dose</t>
-  </si>
-  <si>
     <t>EUA submission withdrawn by Sanofi</t>
   </si>
   <si>
@@ -2481,9 +2454,6 @@
     <t>WHO authorized pandemic vaccine.  Recognized towards immunity in US.  AstraZeneca vaccine non-US WHO authorized tradenames/identifiers include VAXZEVRIA, AZD1222, ChAdOx1 nCoV-19, COVISHIELD</t>
   </si>
   <si>
-    <t>EUA 07/13/2022, 2-dose vaccine. Used to record Novavax vaccines administered in the US and in non-US locations (includes tradenames NUVAXOVID, COVOVAX)</t>
-  </si>
-  <si>
     <t>SARS-COV-2 COVID-19 Viral Vector Non-replicating Non-US Vaccine Product (CONVIDECIA), CanSino Biological Inc./Beijing Institute of Biotechnology</t>
   </si>
   <si>
@@ -2589,39 +2559,24 @@
     <t>SARS-COV-2 (COVID-19) vaccine, mRNA, spike protein, LNP, bivalent, preservative free, 50 mcg/0.5 mL or 25 mcg/0.25 mL dose</t>
   </si>
   <si>
-    <t>EUA updated 04/18/2023 Moderna bivalent dosing (original strain + omicron BA.4/BA.5).  Ages 6 mo and older- dose schedule and dose volume may vary by age and criteria.  Non-US Tradename for same formulation (Spikevax Bivalent) - not authorized by WHO - is authorized by EU and counted toward US immunity</t>
-  </si>
-  <si>
     <t>COVID-19, mRNA, LNP-S, bivalent, PF, 10 mcg/0.2 mL dose</t>
   </si>
   <si>
     <t>SARS-COV-2 (COVID-19) vaccine, mRNA, spike protein, LNP, bivalent, preservative free, 10 mcg/0.2 mL dose, tris-sucrose formulation</t>
   </si>
   <si>
-    <t>EUA updated 4/18/2023 Pfizer bivalent dosing, original strain + omicron BA.4/BA.5. Ages 5 yrs through 11 yrs.</t>
-  </si>
-  <si>
     <t>COVID-19, mRNA, LNP-S, bivalent, PF, 30 mcg/0.3 mL dose</t>
   </si>
   <si>
     <t>SARS-COV-2 (COVID-19) vaccine, mRNA, spike protein, LNP, bivalent, preservative free, 30 mcg/0.3 mL dose, tris-sucrose formulation</t>
   </si>
   <si>
-    <t>EUA updated 4/18/2023 Pfizer bivalent dosing, original strain + omicron BA.4/BA.5. Ages 12 yrs and older. Not Authorized by WHO.  Non-US Tradename for same formulation (Comirnaty Bivalent) counted toward immunity in US</t>
-  </si>
-  <si>
     <t>COVID-19, mRNA, LNP-S, bivalent, PF, 10 mcg/0.2 mL</t>
   </si>
   <si>
     <t>SARS-COV-2 (COVID-19) vaccine, mRNA, spike protein, LNP, bivalent, preservative free, 10 mcg/0.2 mL dose</t>
   </si>
   <si>
-    <t>EUA updated 04/18/2023 Moderna bivalent dosing (original strain + omicron BA.4/BA.5). Ages 6 mo through 5 yrs.</t>
-  </si>
-  <si>
-    <t>EUA updated 4/18/2023 Pfizer bivalent dosing, original + omicron BA.4/BA.5. Ages 6 mo through 4 yrs.</t>
-  </si>
-  <si>
     <t>54</t>
   </si>
   <si>
@@ -2670,12 +2625,6 @@
     <t>RSV, mAb, nirsevimab-alip, 1 mL, neonate to 24 months</t>
   </si>
   <si>
-    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1Îº, (nirsevimab-alip), 0.5 mL, neonates and children to 24 months</t>
-  </si>
-  <si>
-    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1Îº, (nirsevimab-alip), 1 mL, neonates and children to 24 months</t>
-  </si>
-  <si>
     <t>313</t>
   </si>
   <si>
@@ -2743,6 +2692,93 @@
   </si>
   <si>
     <t>Moderna Fall 2023 6 months through 11 years of age</t>
+  </si>
+  <si>
+    <t>Unspecified, for historic records where it is not known if RSV vaccine or RSV MAB was administered</t>
+  </si>
+  <si>
+    <t>315</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) MAB, unspecified</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) monoclonal antibody (MAB), unspecified</t>
+  </si>
+  <si>
+    <t>Unspecified, for historic records where the specific RSV MAB administered is not known</t>
+  </si>
+  <si>
+    <t>314</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) vaccine, unspecified</t>
+  </si>
+  <si>
+    <t>Unspecified, for historic records where the specific vaccine administered is not known</t>
+  </si>
+  <si>
+    <t>Original monovalent Moderna adult vaccine. FDA rescinded all doses for US use 4/18/2023. Continue to used to record historic US Moderna vaccines and those administered in non-US locations (includes tradename Spikevax)</t>
+  </si>
+  <si>
+    <t>Original monovalent Moderna adult vaccine (12+ yrs). FDA rescinded all doses for US use 4/18/2023.  Continue to use to record historic US Pfizer vaccines and Non-US vaccines administered (includes tradename Comirnaty)</t>
+  </si>
+  <si>
+    <t>Original monovalent Janssen/J&amp;J adult vaccine. All NDCs expired 6/20/2023, not reauthorized by FDA for Fall 2023 US doses. Continue to use to record Jansses/J&amp;J Non-US vaccines administered vaccines administered</t>
+  </si>
+  <si>
+    <t>Original monovalent Novavax vaccine (12+ years), FDA rescinded for US doses 10/03/2023. Continue to use to record Novavax Non-US vaccines administered (includes tradenames NUVAXOVID, COVOVAX)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original monovalent Pfizer tris-sucrose formulation (6 mo through 4 yrs), FDA rescinded 4/18/2023 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original monovalent Pfizer tris-sucrose formulation FDA EUA (12+ yrs) and BLA (16+ yrs), FDA rescinded monovalent use 08/31/2022, BLA NDCs not retired until 09/11/2023. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Original monovalent Pfizer tris-sucrose formulation (5 yrs through 11 yrs), FDA rescinded 4/18/2023 </t>
+  </si>
+  <si>
+    <t>Original monovalent Moderna, (Adult) FDA rescinded 4/18/2023, (6 yrs through 11 yrs) FDA rescinded 04/18/2023</t>
+  </si>
+  <si>
+    <t>Original monovalent Moderna pediatric vaccine (FDA rescinded 4/18/2023). Inactivated 6/14/2022 to use CVX code 221 product instead</t>
+  </si>
+  <si>
+    <t>Original monovalent Moderna pediatric vaccine (6 mo through 5 yrs), FDA rescinded 4/18/2023</t>
+  </si>
+  <si>
+    <t>Original strain + omicron BA.4/BA.5 bivalent Moderna vaccine (6 mo and older), FDA rescinded 9/11/2023.  Continue to use to record Non-US vaccines administered (tradename Spikevax Bivalent)</t>
+  </si>
+  <si>
+    <t>Original strain + omicron BA.4/BA.5 bivalent Pfizer vaccine (5 yrs through 11 yrs), FDA rescinded 9/11/2023</t>
+  </si>
+  <si>
+    <t>Original strain + omicron BA.4/BA.5 bivalent Pfizer vaccine (12 yrs and older). FDA rescinded 09/11/2023.  Continue to use to record Non-US vaccines administered (tradename Comirnaty Bivalent)</t>
+  </si>
+  <si>
+    <t>Original strain + omicron BA.4/BA.5 bivalent Moderna vaccine (6 mo through 5 yrs), FDA rescinded 9/11/2023</t>
+  </si>
+  <si>
+    <t>Original strain + omicron BA.4/BA.5 bivalent Pfizer vaccine (6 mo through 4 yrs), FDA rescinded 09/11/2023</t>
+  </si>
+  <si>
+    <t>316</t>
+  </si>
+  <si>
+    <t>meningococcal polysaccharide (MenACWY-TT conjugate), (MenB), PF</t>
+  </si>
+  <si>
+    <t>meningococcal polysaccharide (groups A, C, Y, W) tetanus toxoid conjugate, meningococcal B recombinant vaccine, 0.5mL, preservative free</t>
+  </si>
+  <si>
+    <t>Meningococcal pentavalent vaccine strains ABCW and Y</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ, (nirsevimab-alip), 0.5 mL, neonates and children to 24 months</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ, (nirsevimab-alip), 1 mL, neonates and children to 24 months</t>
   </si>
 </sst>
 </file>
@@ -2750,7 +2786,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -2790,7 +2826,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+      <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2806,7 +2842,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes" connectionId="1" xr16:uid="{7455F197-04B9-4AB9-B953-3A9507690ED2}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes" connectionId="1" xr16:uid="{1631132F-F130-4F3E-9A14-10A24EE86F20}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="11">
     <queryTableFields count="8">
       <queryTableField id="2" name="cvx_code" tableColumnId="2"/>
@@ -2826,16 +2862,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B42541ED-67DA-419F-AA84-58FD1A874578}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" ref="A1:H268" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98AB1904-6AD0-4F39-9CEB-2386DBCF86D7}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" ref="A1:H271" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{07012976-7D71-4EC3-B12C-0091E8B93AAD}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{AE701F1F-6A61-43A4-B24F-67C320BAD2C8}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{F223D56E-6E01-42EA-A411-B574FD16D207}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{3922617F-B752-4F2E-A275-DADD6577F14D}" uniqueName="5" name="Note" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{276E4040-437B-4557-A0D9-0A050FC4F705}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
-    <tableColumn id="1" xr3:uid="{52A2E10B-438F-48E1-96AF-099BC8CAB394}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
-    <tableColumn id="8" xr3:uid="{D6671A33-3BF9-424A-92A1-B80CC3BA2A98}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{4F498A0D-2AAD-4873-BDF2-11F0C8098940}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BCFD0EF8-F19E-4ACF-B2A4-EC3F597C9FDC}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{087CB5D1-4EBF-47C1-8404-15771BB5BF6F}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{715A646E-8E43-433D-A550-5DCFAC5712B5}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{1F0FF025-D7EB-43CF-8BF7-E30C39B36CF5}" uniqueName="5" name="Note" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{88D9561C-EDFF-4270-A7FB-BEB35292F7B0}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{102E658A-B8E0-48DD-B652-2FF46C0FA57E}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
+    <tableColumn id="8" xr3:uid="{BBF6F04F-460E-468D-A0E9-E9F7BF48F1F8}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{F6769F51-B80B-40B3-90B8-44566B8E9953}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3161,29 +3197,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E393B1-1569-412A-AC22-BA5922F95C61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B64273-AC27-48DB-AAE5-059443B1AA84}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I268"/>
+  <dimension ref="A1:H271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
+      <selection activeCell="C261" sqref="C261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="3" max="3" width="82" customWidth="1"/>
     <col min="4" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3208,11 +3244,10 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>863</v>
+        <v>848</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -3235,9 +3270,8 @@
       <c r="H2" s="1">
         <v>40326</v>
       </c>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3262,9 +3296,8 @@
       <c r="H3" s="1">
         <v>40326</v>
       </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -3289,9 +3322,8 @@
       <c r="H4" s="1">
         <v>40451</v>
       </c>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -3316,9 +3348,8 @@
       <c r="H5" s="1">
         <v>43627</v>
       </c>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3343,9 +3374,8 @@
       <c r="H6" s="1">
         <v>40326</v>
       </c>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3370,9 +3400,8 @@
       <c r="H7" s="1">
         <v>44078</v>
       </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -3397,9 +3426,8 @@
       <c r="H8" s="1">
         <v>42538</v>
       </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -3424,20 +3452,19 @@
       <c r="H9" s="1">
         <v>44078</v>
       </c>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
       <c r="C10" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="D10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -3451,9 +3478,8 @@
       <c r="H10" s="1">
         <v>44973</v>
       </c>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -3478,9 +3504,8 @@
       <c r="H11" s="1">
         <v>44078</v>
       </c>
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -3505,9 +3530,8 @@
       <c r="H12" s="1">
         <v>40326</v>
       </c>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -3532,9 +3556,8 @@
       <c r="H13" s="1">
         <v>40326</v>
       </c>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -3559,9 +3582,8 @@
       <c r="H14" s="1">
         <v>40326</v>
       </c>
-      <c r="I14"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -3586,9 +3608,8 @@
       <c r="H15" s="1">
         <v>40451</v>
       </c>
-      <c r="I15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -3613,9 +3634,8 @@
       <c r="H16" s="1">
         <v>40326</v>
       </c>
-      <c r="I16"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -3640,9 +3660,8 @@
       <c r="H17" s="1">
         <v>42814</v>
       </c>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -3667,9 +3686,8 @@
       <c r="H18" s="1">
         <v>40326</v>
       </c>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -3694,9 +3712,8 @@
       <c r="H19" s="1">
         <v>40326</v>
       </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -3721,9 +3738,8 @@
       <c r="H20" s="1">
         <v>40326</v>
       </c>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -3748,9 +3764,8 @@
       <c r="H21" s="1">
         <v>42817</v>
       </c>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -3775,9 +3790,8 @@
       <c r="H22" s="1">
         <v>42510</v>
       </c>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -3802,9 +3816,8 @@
       <c r="H23" s="1">
         <v>44083</v>
       </c>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>115</v>
       </c>
@@ -3829,9 +3842,8 @@
       <c r="H24" s="1">
         <v>40326</v>
       </c>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -3856,9 +3868,8 @@
       <c r="H25" s="1">
         <v>40326</v>
       </c>
-      <c r="I25"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -3883,9 +3894,8 @@
       <c r="H26" s="1">
         <v>40326</v>
       </c>
-      <c r="I26"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>133</v>
       </c>
@@ -3910,9 +3920,8 @@
       <c r="H27" s="1">
         <v>40451</v>
       </c>
-      <c r="I27"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -3937,9 +3946,8 @@
       <c r="H28" s="1">
         <v>40451</v>
       </c>
-      <c r="I28"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3964,9 +3972,8 @@
       <c r="H29" s="1">
         <v>40326</v>
       </c>
-      <c r="I29"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -3991,9 +3998,8 @@
       <c r="H30" s="1">
         <v>44078</v>
       </c>
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -4018,9 +4024,8 @@
       <c r="H31" s="1">
         <v>43230</v>
       </c>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>148</v>
       </c>
@@ -4045,9 +4050,8 @@
       <c r="H32" s="1">
         <v>40326</v>
       </c>
-      <c r="I32"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>152</v>
       </c>
@@ -4072,9 +4076,8 @@
       <c r="H33" s="1">
         <v>43230</v>
       </c>
-      <c r="I33"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -4099,9 +4102,8 @@
       <c r="H34" s="1">
         <v>43593</v>
       </c>
-      <c r="I34"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>158</v>
       </c>
@@ -4126,9 +4128,8 @@
       <c r="H35" s="1">
         <v>40451</v>
       </c>
-      <c r="I35"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -4153,9 +4154,8 @@
       <c r="H36" s="1">
         <v>44083</v>
       </c>
-      <c r="I36"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>165</v>
       </c>
@@ -4180,9 +4180,8 @@
       <c r="H37" s="1">
         <v>44083</v>
       </c>
-      <c r="I37"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>168</v>
       </c>
@@ -4207,9 +4206,8 @@
       <c r="H38" s="1">
         <v>44083</v>
       </c>
-      <c r="I38"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -4234,9 +4232,8 @@
       <c r="H39" s="1">
         <v>40326</v>
       </c>
-      <c r="I39"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>171</v>
       </c>
@@ -4261,9 +4258,8 @@
       <c r="H40" s="1">
         <v>40326</v>
       </c>
-      <c r="I40"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -4288,9 +4284,8 @@
       <c r="H41" s="1">
         <v>40326</v>
       </c>
-      <c r="I41"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>177</v>
       </c>
@@ -4315,9 +4310,8 @@
       <c r="H42" s="1">
         <v>40326</v>
       </c>
-      <c r="I42"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>183</v>
       </c>
@@ -4342,9 +4336,8 @@
       <c r="H43" s="1">
         <v>40451</v>
       </c>
-      <c r="I43"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>186</v>
       </c>
@@ -4369,9 +4362,8 @@
       <c r="H44" s="1">
         <v>42440</v>
       </c>
-      <c r="I44"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>190</v>
       </c>
@@ -4396,9 +4388,8 @@
       <c r="H45" s="1">
         <v>44083</v>
       </c>
-      <c r="I45"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>193</v>
       </c>
@@ -4423,9 +4414,8 @@
       <c r="H46" s="1">
         <v>40326</v>
       </c>
-      <c r="I46"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>196</v>
       </c>
@@ -4450,9 +4440,8 @@
       <c r="H47" s="1">
         <v>43984</v>
       </c>
-      <c r="I47"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>205</v>
       </c>
@@ -4477,9 +4466,8 @@
       <c r="H48" s="1">
         <v>44078</v>
       </c>
-      <c r="I48"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -4504,9 +4492,8 @@
       <c r="H49" s="1">
         <v>44078</v>
       </c>
-      <c r="I49"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>208</v>
       </c>
@@ -4531,9 +4518,8 @@
       <c r="H50" s="1">
         <v>44994</v>
       </c>
-      <c r="I50"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>250</v>
       </c>
@@ -4558,9 +4544,8 @@
       <c r="H51" s="1">
         <v>41904</v>
       </c>
-      <c r="I51"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>272</v>
       </c>
@@ -4585,9 +4570,8 @@
       <c r="H52" s="1">
         <v>40451</v>
       </c>
-      <c r="I52"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>283</v>
       </c>
@@ -4612,9 +4596,8 @@
       <c r="H53" s="1">
         <v>40326</v>
       </c>
-      <c r="I53"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>279</v>
       </c>
@@ -4639,9 +4622,8 @@
       <c r="H54" s="1">
         <v>40451</v>
       </c>
-      <c r="I54"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>221</v>
       </c>
@@ -4666,9 +4648,8 @@
       <c r="H55" s="1">
         <v>40326</v>
       </c>
-      <c r="I55"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>286</v>
       </c>
@@ -4693,9 +4674,8 @@
       <c r="H56" s="1">
         <v>40326</v>
       </c>
-      <c r="I56"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>381</v>
       </c>
@@ -4720,9 +4700,8 @@
       <c r="H57" s="1">
         <v>42776</v>
       </c>
-      <c r="I57"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>426</v>
       </c>
@@ -4747,9 +4726,8 @@
       <c r="H58" s="1">
         <v>40451</v>
       </c>
-      <c r="I58"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>292</v>
       </c>
@@ -4774,9 +4752,8 @@
       <c r="H59" s="1">
         <v>42271</v>
       </c>
-      <c r="I59"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>299</v>
       </c>
@@ -4801,9 +4778,8 @@
       <c r="H60" s="1">
         <v>44083</v>
       </c>
-      <c r="I60"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>302</v>
       </c>
@@ -4828,9 +4804,8 @@
       <c r="H61" s="1">
         <v>44083</v>
       </c>
-      <c r="I61"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>305</v>
       </c>
@@ -4855,9 +4830,8 @@
       <c r="H62" s="1">
         <v>44083</v>
       </c>
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>308</v>
       </c>
@@ -4882,9 +4856,8 @@
       <c r="H63" s="1">
         <v>40326</v>
       </c>
-      <c r="I63"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>359</v>
       </c>
@@ -4909,9 +4882,8 @@
       <c r="H64" s="1">
         <v>40326</v>
       </c>
-      <c r="I64"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>311</v>
       </c>
@@ -4936,9 +4908,8 @@
       <c r="H65" s="1">
         <v>40326</v>
       </c>
-      <c r="I65"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>362</v>
       </c>
@@ -4963,9 +4934,8 @@
       <c r="H66" s="1">
         <v>40326</v>
       </c>
-      <c r="I66"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>314</v>
       </c>
@@ -4990,9 +4960,8 @@
       <c r="H67" s="1">
         <v>44083</v>
       </c>
-      <c r="I67"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>317</v>
       </c>
@@ -5017,9 +4986,8 @@
       <c r="H68" s="1">
         <v>40421</v>
       </c>
-      <c r="I68"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>320</v>
       </c>
@@ -5044,9 +5012,8 @@
       <c r="H69" s="1">
         <v>44083</v>
       </c>
-      <c r="I69"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>352</v>
       </c>
@@ -5071,9 +5038,8 @@
       <c r="H70" s="1">
         <v>43035</v>
       </c>
-      <c r="I70"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>336</v>
       </c>
@@ -5098,9 +5064,8 @@
       <c r="H71" s="1">
         <v>40326</v>
       </c>
-      <c r="I71"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>349</v>
       </c>
@@ -5125,9 +5090,8 @@
       <c r="H72" s="1">
         <v>40326</v>
       </c>
-      <c r="I72"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>323</v>
       </c>
@@ -5152,9 +5116,8 @@
       <c r="H73" s="1">
         <v>42339</v>
       </c>
-      <c r="I73"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>365</v>
       </c>
@@ -5179,9 +5142,8 @@
       <c r="H74" s="1">
         <v>42173</v>
       </c>
-      <c r="I74"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>397</v>
       </c>
@@ -5206,9 +5168,8 @@
       <c r="H75" s="1">
         <v>40326</v>
       </c>
-      <c r="I75"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>404</v>
       </c>
@@ -5233,9 +5194,8 @@
       <c r="H76" s="1">
         <v>40326</v>
       </c>
-      <c r="I76"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>407</v>
       </c>
@@ -5260,9 +5220,8 @@
       <c r="H77" s="1">
         <v>43237</v>
       </c>
-      <c r="I77"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>419</v>
       </c>
@@ -5287,9 +5246,8 @@
       <c r="H78" s="1">
         <v>40326</v>
       </c>
-      <c r="I78"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>413</v>
       </c>
@@ -5314,9 +5272,8 @@
       <c r="H79" s="1">
         <v>41816</v>
       </c>
-      <c r="I79"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>422</v>
       </c>
@@ -5341,9 +5298,8 @@
       <c r="H80" s="1">
         <v>40451</v>
       </c>
-      <c r="I80"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>430</v>
       </c>
@@ -5368,9 +5324,8 @@
       <c r="H81" s="1">
         <v>44083</v>
       </c>
-      <c r="I81"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>442</v>
       </c>
@@ -5395,9 +5350,8 @@
       <c r="H82" s="1">
         <v>42661</v>
       </c>
-      <c r="I82"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>439</v>
       </c>
@@ -5422,9 +5376,8 @@
       <c r="H83" s="1">
         <v>42173</v>
       </c>
-      <c r="I83"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>446</v>
       </c>
@@ -5449,9 +5402,8 @@
       <c r="H84" s="1">
         <v>40451</v>
       </c>
-      <c r="I84"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>450</v>
       </c>
@@ -5476,9 +5428,8 @@
       <c r="H85" s="1">
         <v>44083</v>
       </c>
-      <c r="I85"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>464</v>
       </c>
@@ -5503,9 +5454,8 @@
       <c r="H86" s="1">
         <v>44083</v>
       </c>
-      <c r="I86"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>467</v>
       </c>
@@ -5530,9 +5480,8 @@
       <c r="H87" s="1">
         <v>44078</v>
       </c>
-      <c r="I87"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>470</v>
       </c>
@@ -5557,9 +5506,8 @@
       <c r="H88" s="1">
         <v>40326</v>
       </c>
-      <c r="I88"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>479</v>
       </c>
@@ -5584,9 +5532,8 @@
       <c r="H89" s="1">
         <v>40451</v>
       </c>
-      <c r="I89"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>473</v>
       </c>
@@ -5611,9 +5558,8 @@
       <c r="H90" s="1">
         <v>40326</v>
       </c>
-      <c r="I90"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>476</v>
       </c>
@@ -5638,9 +5584,8 @@
       <c r="H91" s="1">
         <v>40326</v>
       </c>
-      <c r="I91"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>482</v>
       </c>
@@ -5651,7 +5596,7 @@
         <v>484</v>
       </c>
       <c r="D92" t="s">
-        <v>870</v>
+        <v>855</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -5665,9 +5610,8 @@
       <c r="H92" s="1">
         <v>45126</v>
       </c>
-      <c r="I92"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>485</v>
       </c>
@@ -5692,9 +5636,8 @@
       <c r="H93" s="1">
         <v>44078</v>
       </c>
-      <c r="I93"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>491</v>
       </c>
@@ -5719,9 +5662,8 @@
       <c r="H94" s="1">
         <v>42173</v>
       </c>
-      <c r="I94"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>494</v>
       </c>
@@ -5746,9 +5688,8 @@
       <c r="H95" s="1">
         <v>40326</v>
       </c>
-      <c r="I95"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>497</v>
       </c>
@@ -5773,9 +5714,8 @@
       <c r="H96" s="1">
         <v>44994</v>
       </c>
-      <c r="I96"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>507</v>
       </c>
@@ -5800,9 +5740,8 @@
       <c r="H97" s="1">
         <v>43035</v>
       </c>
-      <c r="I97"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>504</v>
       </c>
@@ -5827,9 +5766,8 @@
       <c r="H98" s="1">
         <v>43035</v>
       </c>
-      <c r="I98"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>512</v>
       </c>
@@ -5854,9 +5792,8 @@
       <c r="H99" s="1">
         <v>40326</v>
       </c>
-      <c r="I99"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>518</v>
       </c>
@@ -5881,9 +5818,8 @@
       <c r="H100" s="1">
         <v>42230</v>
       </c>
-      <c r="I100"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>522</v>
       </c>
@@ -5908,9 +5844,8 @@
       <c r="H101" s="1">
         <v>40451</v>
       </c>
-      <c r="I101"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>524</v>
       </c>
@@ -5935,9 +5870,8 @@
       <c r="H102" s="1">
         <v>44624</v>
       </c>
-      <c r="I102"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>525</v>
       </c>
@@ -5962,9 +5896,8 @@
       <c r="H103" s="1">
         <v>44078</v>
       </c>
-      <c r="I103"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>531</v>
       </c>
@@ -5989,9 +5922,8 @@
       <c r="H104" s="1">
         <v>44994</v>
       </c>
-      <c r="I104"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>534</v>
       </c>
@@ -6016,9 +5948,8 @@
       <c r="H105" s="1">
         <v>44994</v>
       </c>
-      <c r="I105"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>537</v>
       </c>
@@ -6043,9 +5974,8 @@
       <c r="H106" s="1">
         <v>44994</v>
       </c>
-      <c r="I106"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>527</v>
       </c>
@@ -6070,9 +6000,8 @@
       <c r="H107" s="1">
         <v>44994</v>
       </c>
-      <c r="I107"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>540</v>
       </c>
@@ -6097,9 +6026,8 @@
       <c r="H108" s="1">
         <v>40326</v>
       </c>
-      <c r="I108"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>551</v>
       </c>
@@ -6124,9 +6052,8 @@
       <c r="H109" s="1">
         <v>40451</v>
       </c>
-      <c r="I109"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>542</v>
       </c>
@@ -6151,9 +6078,8 @@
       <c r="H110" s="1">
         <v>40326</v>
       </c>
-      <c r="I110"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>545</v>
       </c>
@@ -6178,9 +6104,8 @@
       <c r="H111" s="1">
         <v>42229</v>
       </c>
-      <c r="I111"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>548</v>
       </c>
@@ -6205,9 +6130,8 @@
       <c r="H112" s="1">
         <v>42173</v>
       </c>
-      <c r="I112"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>555</v>
       </c>
@@ -6232,9 +6156,8 @@
       <c r="H113" s="1">
         <v>40326</v>
       </c>
-      <c r="I113"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>561</v>
       </c>
@@ -6259,9 +6182,8 @@
       <c r="H114" s="1">
         <v>40326</v>
       </c>
-      <c r="I114"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>564</v>
       </c>
@@ -6286,9 +6208,8 @@
       <c r="H115" s="1">
         <v>40326</v>
       </c>
-      <c r="I115"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>567</v>
       </c>
@@ -6313,9 +6234,8 @@
       <c r="H116" s="1">
         <v>44078</v>
       </c>
-      <c r="I116"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>569</v>
       </c>
@@ -6340,9 +6260,8 @@
       <c r="H117" s="1">
         <v>40326</v>
       </c>
-      <c r="I117"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>572</v>
       </c>
@@ -6367,9 +6286,8 @@
       <c r="H118" s="1">
         <v>40326</v>
       </c>
-      <c r="I118"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>575</v>
       </c>
@@ -6394,9 +6312,8 @@
       <c r="H119" s="1">
         <v>40326</v>
       </c>
-      <c r="I119"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>578</v>
       </c>
@@ -6421,9 +6338,8 @@
       <c r="H120" s="1">
         <v>40451</v>
       </c>
-      <c r="I120"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>582</v>
       </c>
@@ -6448,9 +6364,8 @@
       <c r="H121" s="1">
         <v>44078</v>
       </c>
-      <c r="I121"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>585</v>
       </c>
@@ -6475,9 +6390,8 @@
       <c r="H122" s="1">
         <v>44083</v>
       </c>
-      <c r="I122"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>588</v>
       </c>
@@ -6502,9 +6416,8 @@
       <c r="H123" s="1">
         <v>42796</v>
       </c>
-      <c r="I123"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>599</v>
       </c>
@@ -6529,9 +6442,8 @@
       <c r="H124" s="1">
         <v>40326</v>
       </c>
-      <c r="I124"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>8</v>
       </c>
@@ -6556,9 +6468,8 @@
       <c r="H125" s="1">
         <v>44994</v>
       </c>
-      <c r="I125"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>15</v>
       </c>
@@ -6583,9 +6494,8 @@
       <c r="H126" s="1">
         <v>44131</v>
       </c>
-      <c r="I126"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>12</v>
       </c>
@@ -6610,9 +6520,8 @@
       <c r="H127" s="1">
         <v>44083</v>
       </c>
-      <c r="I127"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -6637,9 +6546,8 @@
       <c r="H128" s="1">
         <v>40326</v>
       </c>
-      <c r="I128"/>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>289</v>
       </c>
@@ -6664,9 +6572,8 @@
       <c r="H129" s="1">
         <v>40326</v>
       </c>
-      <c r="I129"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>199</v>
       </c>
@@ -6691,9 +6598,8 @@
       <c r="H130" s="1">
         <v>40451</v>
       </c>
-      <c r="I130"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>346</v>
       </c>
@@ -6718,9 +6624,8 @@
       <c r="H131" s="1">
         <v>40326</v>
       </c>
-      <c r="I131"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>224</v>
       </c>
@@ -6745,9 +6650,8 @@
       <c r="H132" s="1">
         <v>40326</v>
       </c>
-      <c r="I132"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>558</v>
       </c>
@@ -6772,9 +6676,8 @@
       <c r="H133" s="1">
         <v>40326</v>
       </c>
-      <c r="I133"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>96</v>
       </c>
@@ -6799,9 +6702,8 @@
       <c r="H134" s="1">
         <v>43230</v>
       </c>
-      <c r="I134"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>371</v>
       </c>
@@ -6826,9 +6728,8 @@
       <c r="H135" s="1">
         <v>40418</v>
       </c>
-      <c r="I135"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>375</v>
       </c>
@@ -6853,9 +6754,8 @@
       <c r="H136" s="1">
         <v>40418</v>
       </c>
-      <c r="I136"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>378</v>
       </c>
@@ -6880,9 +6780,8 @@
       <c r="H137" s="1">
         <v>40418</v>
       </c>
-      <c r="I137"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>368</v>
       </c>
@@ -6907,9 +6806,8 @@
       <c r="H138" s="1">
         <v>40418</v>
       </c>
-      <c r="I138"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>500</v>
       </c>
@@ -6934,9 +6832,8 @@
       <c r="H139" s="1">
         <v>40451</v>
       </c>
-      <c r="I139"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>510</v>
       </c>
@@ -6961,9 +6858,8 @@
       <c r="H140" s="1">
         <v>43704</v>
       </c>
-      <c r="I140"/>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>267</v>
       </c>
@@ -6974,7 +6870,7 @@
         <v>268</v>
       </c>
       <c r="D141" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
       <c r="E141" t="s">
         <v>11</v>
@@ -6988,9 +6884,8 @@
       <c r="H141" s="1">
         <v>44910</v>
       </c>
-      <c r="I141"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>295</v>
       </c>
@@ -7015,9 +6910,8 @@
       <c r="H142" s="1">
         <v>40451</v>
       </c>
-      <c r="I142"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>264</v>
       </c>
@@ -7042,9 +6936,8 @@
       <c r="H143" s="1">
         <v>41472</v>
       </c>
-      <c r="I143"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>520</v>
       </c>
@@ -7069,9 +6962,8 @@
       <c r="H144" s="1">
         <v>42230</v>
       </c>
-      <c r="I144"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>19</v>
       </c>
@@ -7096,9 +6988,8 @@
       <c r="H145" s="1">
         <v>40622</v>
       </c>
-      <c r="I145"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>269</v>
       </c>
@@ -7109,7 +7000,7 @@
         <v>271</v>
       </c>
       <c r="D146" t="s">
-        <v>830</v>
+        <v>820</v>
       </c>
       <c r="E146" t="s">
         <v>11</v>
@@ -7123,9 +7014,8 @@
       <c r="H146" s="1">
         <v>44910</v>
       </c>
-      <c r="I146"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>488</v>
       </c>
@@ -7150,9 +7040,8 @@
       <c r="H147" s="1">
         <v>44083</v>
       </c>
-      <c r="I147"/>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>77</v>
       </c>
@@ -7163,7 +7052,7 @@
         <v>79</v>
       </c>
       <c r="D148" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -7177,9 +7066,8 @@
       <c r="H148" s="1">
         <v>44783</v>
       </c>
-      <c r="I148"/>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>342</v>
       </c>
@@ -7204,9 +7092,8 @@
       <c r="H149" s="1">
         <v>40947</v>
       </c>
-      <c r="I149"/>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>339</v>
       </c>
@@ -7231,9 +7118,8 @@
       <c r="H150" s="1">
         <v>43231</v>
       </c>
-      <c r="I150"/>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>254</v>
       </c>
@@ -7258,9 +7144,8 @@
       <c r="H151" s="1">
         <v>41472</v>
       </c>
-      <c r="I151"/>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>241</v>
       </c>
@@ -7285,9 +7170,8 @@
       <c r="H152" s="1">
         <v>41472</v>
       </c>
-      <c r="I152"/>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>218</v>
       </c>
@@ -7312,9 +7196,8 @@
       <c r="H153" s="1">
         <v>41302</v>
       </c>
-      <c r="I153"/>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>416</v>
       </c>
@@ -7339,9 +7222,8 @@
       <c r="H154" s="1">
         <v>41302</v>
       </c>
-      <c r="I154"/>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>227</v>
       </c>
@@ -7366,9 +7248,8 @@
       <c r="H155" s="1">
         <v>42545</v>
       </c>
-      <c r="I155"/>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>118</v>
       </c>
@@ -7393,9 +7274,8 @@
       <c r="H156" s="1">
         <v>44083</v>
       </c>
-      <c r="I156"/>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>257</v>
       </c>
@@ -7420,9 +7300,8 @@
       <c r="H157" s="1">
         <v>41472</v>
       </c>
-      <c r="I157"/>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>460</v>
       </c>
@@ -7447,9 +7326,8 @@
       <c r="H158" s="1">
         <v>44078</v>
       </c>
-      <c r="I158"/>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>456</v>
       </c>
@@ -7474,9 +7352,8 @@
       <c r="H159" s="1">
         <v>44078</v>
       </c>
-      <c r="I159"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>237</v>
       </c>
@@ -7501,9 +7378,8 @@
       <c r="H160" s="1">
         <v>41506</v>
       </c>
-      <c r="I160"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>453</v>
       </c>
@@ -7528,9 +7404,8 @@
       <c r="H161" s="1">
         <v>44994</v>
       </c>
-      <c r="I161"/>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>214</v>
       </c>
@@ -7555,9 +7430,8 @@
       <c r="H162" s="1">
         <v>41786</v>
       </c>
-      <c r="I162"/>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>39</v>
       </c>
@@ -7582,9 +7456,8 @@
       <c r="H163" s="1">
         <v>44131</v>
       </c>
-      <c r="I163"/>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>245</v>
       </c>
@@ -7609,9 +7482,8 @@
       <c r="H164" s="1">
         <v>41843</v>
       </c>
-      <c r="I164"/>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>330</v>
       </c>
@@ -7636,9 +7508,8 @@
       <c r="H165" s="1">
         <v>41946</v>
       </c>
-      <c r="I165"/>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>327</v>
       </c>
@@ -7663,9 +7534,8 @@
       <c r="H166" s="1">
         <v>42037</v>
       </c>
-      <c r="I166"/>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>333</v>
       </c>
@@ -7690,9 +7560,8 @@
       <c r="H167" s="1">
         <v>41946</v>
       </c>
-      <c r="I167"/>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>202</v>
       </c>
@@ -7717,9 +7586,8 @@
       <c r="H168" s="1">
         <v>41984</v>
       </c>
-      <c r="I168"/>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>247</v>
       </c>
@@ -7730,7 +7598,7 @@
         <v>249</v>
       </c>
       <c r="D169" t="s">
-        <v>831</v>
+        <v>821</v>
       </c>
       <c r="E169" t="s">
         <v>11</v>
@@ -7744,9 +7612,8 @@
       <c r="H169" s="1">
         <v>44910</v>
       </c>
-      <c r="I169"/>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>355</v>
       </c>
@@ -7771,9 +7638,8 @@
       <c r="H170" s="1">
         <v>42339</v>
       </c>
-      <c r="I170"/>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>276</v>
       </c>
@@ -7798,9 +7664,8 @@
       <c r="H171" s="1">
         <v>42348</v>
       </c>
-      <c r="I171"/>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>122</v>
       </c>
@@ -7825,9 +7690,8 @@
       <c r="H172" s="1">
         <v>42500</v>
       </c>
-      <c r="I172"/>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>80</v>
       </c>
@@ -7852,9 +7716,8 @@
       <c r="H173" s="1">
         <v>42510</v>
       </c>
-      <c r="I173"/>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>231</v>
       </c>
@@ -7879,9 +7742,8 @@
       <c r="H174" s="1">
         <v>42537</v>
       </c>
-      <c r="I174"/>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>55</v>
       </c>
@@ -7906,9 +7768,8 @@
       <c r="H175" s="1">
         <v>42538</v>
       </c>
-      <c r="I175"/>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>47</v>
       </c>
@@ -7933,9 +7794,8 @@
       <c r="H176" s="1">
         <v>42538</v>
       </c>
-      <c r="I176"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>50</v>
       </c>
@@ -7960,9 +7820,8 @@
       <c r="H177" s="1">
         <v>42538</v>
       </c>
-      <c r="I177"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>433</v>
       </c>
@@ -7987,9 +7846,8 @@
       <c r="H178" s="1">
         <v>42661</v>
       </c>
-      <c r="I178"/>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>436</v>
       </c>
@@ -8014,9 +7872,8 @@
       <c r="H179" s="1">
         <v>42661</v>
       </c>
-      <c r="I179"/>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>400</v>
       </c>
@@ -8041,9 +7898,8 @@
       <c r="H180" s="1">
         <v>42723</v>
       </c>
-      <c r="I180"/>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>389</v>
       </c>
@@ -8068,9 +7924,8 @@
       <c r="H181" s="1">
         <v>42752</v>
       </c>
-      <c r="I181"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>385</v>
       </c>
@@ -8095,9 +7950,8 @@
       <c r="H182" s="1">
         <v>42752</v>
       </c>
-      <c r="I182"/>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>515</v>
       </c>
@@ -8122,9 +7976,8 @@
       <c r="H183" s="1">
         <v>44083</v>
       </c>
-      <c r="I183"/>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>37</v>
       </c>
@@ -8149,9 +8002,8 @@
       <c r="H184" s="1">
         <v>44078</v>
       </c>
-      <c r="I184"/>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>393</v>
       </c>
@@ -8176,9 +8028,8 @@
       <c r="H185" s="1">
         <v>42752</v>
       </c>
-      <c r="I185"/>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>592</v>
       </c>
@@ -8203,9 +8054,8 @@
       <c r="H186" s="1">
         <v>42796</v>
       </c>
-      <c r="I186"/>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>596</v>
       </c>
@@ -8230,9 +8080,8 @@
       <c r="H187" s="1">
         <v>42796</v>
       </c>
-      <c r="I187"/>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>261</v>
       </c>
@@ -8257,9 +8106,8 @@
       <c r="H188" s="1">
         <v>42846</v>
       </c>
-      <c r="I188"/>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>234</v>
       </c>
@@ -8284,9 +8132,8 @@
       <c r="H189" s="1">
         <v>42913</v>
       </c>
-      <c r="I189"/>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>602</v>
       </c>
@@ -8311,9 +8158,8 @@
       <c r="H190" s="1">
         <v>43035</v>
       </c>
-      <c r="I190"/>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>605</v>
       </c>
@@ -8338,9 +8184,8 @@
       <c r="H191" s="1">
         <v>43035</v>
       </c>
-      <c r="I191"/>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>144</v>
       </c>
@@ -8365,9 +8210,8 @@
       <c r="H192" s="1">
         <v>43230</v>
       </c>
-      <c r="I192"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>616</v>
       </c>
@@ -8392,9 +8236,8 @@
       <c r="H193" s="1">
         <v>44943</v>
       </c>
-      <c r="I193"/>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>619</v>
       </c>
@@ -8419,9 +8262,8 @@
       <c r="H194" s="1">
         <v>43230</v>
       </c>
-      <c r="I194"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>622</v>
       </c>
@@ -8446,9 +8288,8 @@
       <c r="H195" s="1">
         <v>43230</v>
       </c>
-      <c r="I195"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>625</v>
       </c>
@@ -8473,9 +8314,8 @@
       <c r="H196" s="1">
         <v>43333</v>
       </c>
-      <c r="I196"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>629</v>
       </c>
@@ -8500,9 +8340,8 @@
       <c r="H197" s="1">
         <v>44028</v>
       </c>
-      <c r="I197"/>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>632</v>
       </c>
@@ -8527,9 +8366,8 @@
       <c r="H198" s="1">
         <v>44943</v>
       </c>
-      <c r="I198"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>636</v>
       </c>
@@ -8554,9 +8392,8 @@
       <c r="H199" s="1">
         <v>43692</v>
       </c>
-      <c r="I199"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>641</v>
       </c>
@@ -8564,7 +8401,7 @@
         <v>642</v>
       </c>
       <c r="C200" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
       <c r="D200" t="s">
         <v>661</v>
@@ -8581,9 +8418,8 @@
       <c r="H200" s="1">
         <v>44943</v>
       </c>
-      <c r="I200"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>643</v>
       </c>
@@ -8608,9 +8444,8 @@
       <c r="H201" s="1">
         <v>44943</v>
       </c>
-      <c r="I201"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>647</v>
       </c>
@@ -8635,9 +8470,8 @@
       <c r="H202" s="1">
         <v>44943</v>
       </c>
-      <c r="I202"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>651</v>
       </c>
@@ -8662,9 +8496,8 @@
       <c r="H203" s="1">
         <v>44943</v>
       </c>
-      <c r="I203"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>655</v>
       </c>
@@ -8689,17 +8522,16 @@
       <c r="H204" s="1">
         <v>44943</v>
       </c>
-      <c r="I204"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>662</v>
       </c>
       <c r="B205" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="C205" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="D205" t="s">
         <v>26</v>
@@ -8716,9 +8548,8 @@
       <c r="H205" s="1">
         <v>44952</v>
       </c>
-      <c r="I205"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>663</v>
       </c>
@@ -8726,7 +8557,7 @@
         <v>664</v>
       </c>
       <c r="C206" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="D206" t="s">
         <v>26</v>
@@ -8743,20 +8574,19 @@
       <c r="H206" s="1">
         <v>44943</v>
       </c>
-      <c r="I206"/>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>665</v>
       </c>
       <c r="B207" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
       <c r="C207" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D207" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E207" t="s">
         <v>23</v>
@@ -8770,9 +8600,8 @@
       <c r="H207" s="1">
         <v>44971</v>
       </c>
-      <c r="I207"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>666</v>
       </c>
@@ -8783,10 +8612,10 @@
         <v>741</v>
       </c>
       <c r="D208" t="s">
-        <v>803</v>
+        <v>895</v>
       </c>
       <c r="E208" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F208">
         <v>230</v>
@@ -8795,11 +8624,10 @@
         <v>609</v>
       </c>
       <c r="H208" s="1">
-        <v>44811</v>
-      </c>
-      <c r="I208"/>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>667</v>
       </c>
@@ -8810,10 +8638,10 @@
         <v>669</v>
       </c>
       <c r="D209" t="s">
-        <v>804</v>
+        <v>896</v>
       </c>
       <c r="E209" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F209">
         <v>231</v>
@@ -8822,11 +8650,10 @@
         <v>609</v>
       </c>
       <c r="H209" s="1">
-        <v>44811</v>
-      </c>
-      <c r="I209"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>671</v>
       </c>
@@ -8851,9 +8678,8 @@
       <c r="H210" s="1">
         <v>44408</v>
       </c>
-      <c r="I210"/>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>672</v>
       </c>
@@ -8864,7 +8690,7 @@
         <v>674</v>
       </c>
       <c r="D211" t="s">
-        <v>815</v>
+        <v>806</v>
       </c>
       <c r="E211" t="s">
         <v>49</v>
@@ -8878,9 +8704,8 @@
       <c r="H211" s="1">
         <v>44881</v>
       </c>
-      <c r="I211"/>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>675</v>
       </c>
@@ -8891,10 +8716,10 @@
         <v>677</v>
       </c>
       <c r="D212" t="s">
-        <v>749</v>
+        <v>897</v>
       </c>
       <c r="E212" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F212">
         <v>234</v>
@@ -8903,11 +8728,10 @@
         <v>609</v>
       </c>
       <c r="H212" s="1">
-        <v>44447</v>
-      </c>
-      <c r="I212"/>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>678</v>
       </c>
@@ -8918,7 +8742,7 @@
         <v>680</v>
       </c>
       <c r="D213" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="E213" t="s">
         <v>23</v>
@@ -8932,9 +8756,8 @@
       <c r="H213" s="1">
         <v>44938</v>
       </c>
-      <c r="I213"/>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>681</v>
       </c>
@@ -8959,23 +8782,22 @@
       <c r="H214" s="1">
         <v>44292</v>
       </c>
-      <c r="I214"/>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>683</v>
       </c>
       <c r="B215" t="s">
+        <v>749</v>
+      </c>
+      <c r="C215" t="s">
         <v>750</v>
       </c>
-      <c r="C215" t="s">
-        <v>751</v>
-      </c>
       <c r="D215" t="s">
-        <v>816</v>
+        <v>898</v>
       </c>
       <c r="E215" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F215">
         <v>237</v>
@@ -8984,11 +8806,10 @@
         <v>609</v>
       </c>
       <c r="H215" s="1">
-        <v>44894</v>
-      </c>
-      <c r="I215"/>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45223</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>685</v>
       </c>
@@ -9013,9 +8834,8 @@
       <c r="H216" s="1">
         <v>44392</v>
       </c>
-      <c r="I216"/>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>689</v>
       </c>
@@ -9040,9 +8860,8 @@
       <c r="H217" s="1">
         <v>44392</v>
       </c>
-      <c r="I217"/>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>693</v>
       </c>
@@ -9067,9 +8886,8 @@
       <c r="H218" s="1">
         <v>44519</v>
       </c>
-      <c r="I218"/>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>697</v>
       </c>
@@ -9094,9 +8912,8 @@
       <c r="H219" s="1">
         <v>44392</v>
       </c>
-      <c r="I219"/>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>700</v>
       </c>
@@ -9121,9 +8938,8 @@
       <c r="H220" s="1">
         <v>44392</v>
       </c>
-      <c r="I220"/>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>703</v>
       </c>
@@ -9148,20 +8964,19 @@
       <c r="H221" s="1">
         <v>44392</v>
       </c>
-      <c r="I221"/>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>706</v>
       </c>
       <c r="B222" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="C222" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="D222" t="s">
-        <v>818</v>
+        <v>808</v>
       </c>
       <c r="E222" t="s">
         <v>49</v>
@@ -9175,9 +8990,8 @@
       <c r="H222" s="1">
         <v>44911</v>
       </c>
-      <c r="I222"/>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>707</v>
       </c>
@@ -9202,9 +9016,8 @@
       <c r="H223" s="1">
         <v>44426</v>
       </c>
-      <c r="I223"/>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>709</v>
       </c>
@@ -9229,9 +9042,8 @@
       <c r="H224" s="1">
         <v>44392</v>
       </c>
-      <c r="I224"/>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>712</v>
       </c>
@@ -9256,9 +9068,8 @@
       <c r="H225" s="1">
         <v>44392</v>
       </c>
-      <c r="I225"/>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>715</v>
       </c>
@@ -9269,7 +9080,7 @@
         <v>717</v>
       </c>
       <c r="D226" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="E226" t="s">
         <v>49</v>
@@ -9283,9 +9094,8 @@
       <c r="H226" s="1">
         <v>44880</v>
       </c>
-      <c r="I226"/>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>718</v>
       </c>
@@ -9296,7 +9106,7 @@
         <v>720</v>
       </c>
       <c r="D227" t="s">
-        <v>819</v>
+        <v>809</v>
       </c>
       <c r="E227" t="s">
         <v>49</v>
@@ -9310,9 +9120,8 @@
       <c r="H227" s="1">
         <v>44880</v>
       </c>
-      <c r="I227"/>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>722</v>
       </c>
@@ -9337,9 +9146,8 @@
       <c r="H228" s="1">
         <v>44426</v>
       </c>
-      <c r="I228"/>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>725</v>
       </c>
@@ -9364,9 +9172,8 @@
       <c r="H229" s="1">
         <v>44994</v>
       </c>
-      <c r="I229"/>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>728</v>
       </c>
@@ -9377,10 +9184,10 @@
         <v>730</v>
       </c>
       <c r="D230" t="s">
-        <v>805</v>
+        <v>899</v>
       </c>
       <c r="E230" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F230">
         <v>252</v>
@@ -9389,11 +9196,10 @@
         <v>609</v>
       </c>
       <c r="H230" s="1">
-        <v>44810</v>
-      </c>
-      <c r="I230"/>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>731</v>
       </c>
@@ -9404,10 +9210,10 @@
         <v>733</v>
       </c>
       <c r="D231" t="s">
-        <v>806</v>
+        <v>900</v>
       </c>
       <c r="E231" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F231">
         <v>253</v>
@@ -9416,11 +9222,10 @@
         <v>609</v>
       </c>
       <c r="H231" s="1">
-        <v>44943</v>
-      </c>
-      <c r="I231"/>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45232</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>734</v>
       </c>
@@ -9431,10 +9236,10 @@
         <v>736</v>
       </c>
       <c r="D232" t="s">
-        <v>807</v>
+        <v>901</v>
       </c>
       <c r="E232" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F232">
         <v>254</v>
@@ -9443,11 +9248,10 @@
         <v>609</v>
       </c>
       <c r="H232" s="1">
-        <v>44943</v>
-      </c>
-      <c r="I232"/>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45224</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>738</v>
       </c>
@@ -9472,9 +9276,8 @@
       <c r="H233" s="1">
         <v>44606</v>
       </c>
-      <c r="I233"/>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>744</v>
       </c>
@@ -9485,10 +9288,10 @@
         <v>746</v>
       </c>
       <c r="D234" t="s">
-        <v>808</v>
+        <v>902</v>
       </c>
       <c r="E234" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F234">
         <v>256</v>
@@ -9497,22 +9300,21 @@
         <v>609</v>
       </c>
       <c r="H234" s="1">
-        <v>44811</v>
-      </c>
-      <c r="I234"/>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45224</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
+        <v>751</v>
+      </c>
+      <c r="B235" t="s">
+        <v>767</v>
+      </c>
+      <c r="C235" t="s">
+        <v>768</v>
+      </c>
+      <c r="D235" t="s">
         <v>752</v>
-      </c>
-      <c r="B235" t="s">
-        <v>768</v>
-      </c>
-      <c r="C235" t="s">
-        <v>769</v>
-      </c>
-      <c r="D235" t="s">
-        <v>753</v>
       </c>
       <c r="E235" t="s">
         <v>11</v>
@@ -9526,20 +9328,19 @@
       <c r="H235" s="1">
         <v>44636</v>
       </c>
-      <c r="I235"/>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
+        <v>753</v>
+      </c>
+      <c r="B236" t="s">
         <v>754</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
         <v>755</v>
       </c>
-      <c r="C236" t="s">
+      <c r="D236" t="s">
         <v>756</v>
-      </c>
-      <c r="D236" t="s">
-        <v>757</v>
       </c>
       <c r="E236" t="s">
         <v>23</v>
@@ -9553,20 +9354,19 @@
       <c r="H236" s="1">
         <v>44623</v>
       </c>
-      <c r="I236"/>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
+        <v>757</v>
+      </c>
+      <c r="B237" t="s">
         <v>758</v>
       </c>
-      <c r="B237" t="s">
+      <c r="C237" t="s">
         <v>759</v>
       </c>
-      <c r="C237" t="s">
+      <c r="D237" t="s">
         <v>760</v>
-      </c>
-      <c r="D237" t="s">
-        <v>761</v>
       </c>
       <c r="E237" t="s">
         <v>23</v>
@@ -9580,20 +9380,19 @@
       <c r="H237" s="1">
         <v>44624</v>
       </c>
-      <c r="I237"/>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
+        <v>761</v>
+      </c>
+      <c r="B238" t="s">
         <v>762</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>763</v>
       </c>
-      <c r="C238" t="s">
-        <v>764</v>
-      </c>
       <c r="D238" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="E238" t="s">
         <v>61</v>
@@ -9607,20 +9406,19 @@
       <c r="H238" s="1">
         <v>44994</v>
       </c>
-      <c r="I238"/>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>764</v>
+      </c>
+      <c r="B239" t="s">
         <v>765</v>
       </c>
-      <c r="B239" t="s">
+      <c r="C239" t="s">
         <v>766</v>
       </c>
-      <c r="C239" t="s">
-        <v>767</v>
-      </c>
       <c r="D239" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="E239" t="s">
         <v>61</v>
@@ -9634,20 +9432,19 @@
       <c r="H239" s="1">
         <v>44994</v>
       </c>
-      <c r="I239"/>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
+        <v>769</v>
+      </c>
+      <c r="B240" t="s">
         <v>770</v>
       </c>
-      <c r="B240" t="s">
+      <c r="C240" t="s">
         <v>771</v>
       </c>
-      <c r="C240" t="s">
+      <c r="D240" t="s">
         <v>772</v>
-      </c>
-      <c r="D240" t="s">
-        <v>773</v>
       </c>
       <c r="E240" t="s">
         <v>49</v>
@@ -9661,17 +9458,16 @@
       <c r="H240" s="1">
         <v>44663</v>
       </c>
-      <c r="I240"/>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
+        <v>773</v>
+      </c>
+      <c r="B241" t="s">
         <v>774</v>
       </c>
-      <c r="B241" t="s">
+      <c r="C241" t="s">
         <v>775</v>
-      </c>
-      <c r="C241" t="s">
-        <v>776</v>
       </c>
       <c r="D241" t="s">
         <v>696</v>
@@ -9688,17 +9484,16 @@
       <c r="H241" s="1">
         <v>44663</v>
       </c>
-      <c r="I241"/>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
+        <v>776</v>
+      </c>
+      <c r="B242" t="s">
         <v>777</v>
       </c>
-      <c r="B242" t="s">
+      <c r="C242" t="s">
         <v>778</v>
-      </c>
-      <c r="C242" t="s">
-        <v>779</v>
       </c>
       <c r="D242" t="s">
         <v>696</v>
@@ -9715,17 +9510,16 @@
       <c r="H242" s="1">
         <v>44663</v>
       </c>
-      <c r="I242"/>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
+        <v>779</v>
+      </c>
+      <c r="B243" t="s">
         <v>780</v>
       </c>
-      <c r="B243" t="s">
+      <c r="C243" t="s">
         <v>781</v>
-      </c>
-      <c r="C243" t="s">
-        <v>782</v>
       </c>
       <c r="D243" t="s">
         <v>696</v>
@@ -9742,17 +9536,16 @@
       <c r="H243" s="1">
         <v>44663</v>
       </c>
-      <c r="I243"/>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
+        <v>782</v>
+      </c>
+      <c r="B244" t="s">
         <v>783</v>
       </c>
-      <c r="B244" t="s">
+      <c r="C244" t="s">
         <v>784</v>
-      </c>
-      <c r="C244" t="s">
-        <v>785</v>
       </c>
       <c r="D244" t="s">
         <v>696</v>
@@ -9769,17 +9562,16 @@
       <c r="H244" s="1">
         <v>44663</v>
       </c>
-      <c r="I244"/>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
+        <v>785</v>
+      </c>
+      <c r="B245" t="s">
         <v>786</v>
       </c>
-      <c r="B245" t="s">
+      <c r="C245" t="s">
         <v>787</v>
-      </c>
-      <c r="C245" t="s">
-        <v>788</v>
       </c>
       <c r="D245" t="s">
         <v>696</v>
@@ -9796,20 +9588,19 @@
       <c r="H245" s="1">
         <v>44663</v>
       </c>
-      <c r="I245"/>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>788</v>
+      </c>
+      <c r="B246" t="s">
         <v>789</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C246" t="s">
         <v>790</v>
       </c>
-      <c r="C246" t="s">
-        <v>791</v>
-      </c>
       <c r="D246" t="s">
-        <v>796</v>
+        <v>903</v>
       </c>
       <c r="E246" t="s">
         <v>11</v>
@@ -9821,25 +9612,24 @@
         <v>609</v>
       </c>
       <c r="H246" s="1">
-        <v>44727</v>
-      </c>
-      <c r="I246"/>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
+        <v>791</v>
+      </c>
+      <c r="B247" t="s">
         <v>792</v>
       </c>
-      <c r="B247" t="s">
+      <c r="C247" t="s">
         <v>793</v>
       </c>
-      <c r="C247" t="s">
-        <v>794</v>
-      </c>
       <c r="D247" t="s">
-        <v>809</v>
+        <v>904</v>
       </c>
       <c r="E247" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F247">
         <v>269</v>
@@ -9848,25 +9638,24 @@
         <v>609</v>
       </c>
       <c r="H247" s="1">
-        <v>44810</v>
-      </c>
-      <c r="I247"/>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B248" t="s">
-        <v>850</v>
+        <v>840</v>
       </c>
       <c r="C248" t="s">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="D248" t="s">
-        <v>852</v>
+        <v>905</v>
       </c>
       <c r="E248" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F248">
         <v>270</v>
@@ -9875,25 +9664,24 @@
         <v>609</v>
       </c>
       <c r="H248" s="1">
-        <v>45034</v>
-      </c>
-      <c r="I248"/>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B249" t="s">
-        <v>853</v>
+        <v>842</v>
       </c>
       <c r="C249" t="s">
-        <v>854</v>
+        <v>843</v>
       </c>
       <c r="D249" t="s">
-        <v>855</v>
+        <v>906</v>
       </c>
       <c r="E249" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F249">
         <v>271</v>
@@ -9902,25 +9690,24 @@
         <v>609</v>
       </c>
       <c r="H249" s="1">
-        <v>45034</v>
-      </c>
-      <c r="I249"/>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B250" t="s">
-        <v>856</v>
+        <v>844</v>
       </c>
       <c r="C250" t="s">
-        <v>857</v>
+        <v>845</v>
       </c>
       <c r="D250" t="s">
-        <v>858</v>
+        <v>907</v>
       </c>
       <c r="E250" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F250">
         <v>272</v>
@@ -9929,25 +9716,24 @@
         <v>609</v>
       </c>
       <c r="H250" s="1">
-        <v>45034</v>
-      </c>
-      <c r="I250"/>
-    </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="B251" t="s">
-        <v>859</v>
+        <v>846</v>
       </c>
       <c r="C251" t="s">
-        <v>860</v>
+        <v>847</v>
       </c>
       <c r="D251" t="s">
-        <v>861</v>
+        <v>908</v>
       </c>
       <c r="E251" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F251">
         <v>273</v>
@@ -9956,19 +9742,18 @@
         <v>609</v>
       </c>
       <c r="H251" s="1">
-        <v>45034</v>
-      </c>
-      <c r="I251"/>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="B252" t="s">
-        <v>821</v>
+        <v>811</v>
       </c>
       <c r="C252" t="s">
-        <v>822</v>
+        <v>812</v>
       </c>
       <c r="D252" t="s">
         <v>696</v>
@@ -9985,20 +9770,19 @@
       <c r="H252" s="1">
         <v>44882</v>
       </c>
-      <c r="I252"/>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="B253" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="C253" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="D253" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="E253" t="s">
         <v>49</v>
@@ -10012,20 +9796,19 @@
       <c r="H253" s="1">
         <v>44882</v>
       </c>
-      <c r="I253"/>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="B254" t="s">
-        <v>833</v>
+        <v>823</v>
       </c>
       <c r="C254" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="D254" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="E254" t="s">
         <v>49</v>
@@ -10039,17 +9822,16 @@
       <c r="H254" s="1">
         <v>44914</v>
       </c>
-      <c r="I254"/>
-    </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="B255" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="C255" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="D255" t="s">
         <v>696</v>
@@ -10066,20 +9848,19 @@
       <c r="H255" s="1">
         <v>44979</v>
       </c>
-      <c r="I255"/>
-    </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>846</v>
+        <v>836</v>
       </c>
       <c r="B256" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="C256" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="D256" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="E256" t="s">
         <v>23</v>
@@ -10093,20 +9874,19 @@
       <c r="H256" s="1">
         <v>44999</v>
       </c>
-      <c r="I256"/>
-    </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>864</v>
+        <v>849</v>
       </c>
       <c r="B257" t="s">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="C257" t="s">
-        <v>866</v>
+        <v>851</v>
       </c>
       <c r="D257" t="s">
-        <v>867</v>
+        <v>852</v>
       </c>
       <c r="E257" t="s">
         <v>23</v>
@@ -10120,20 +9900,19 @@
       <c r="H257" s="1">
         <v>45083</v>
       </c>
-      <c r="I257"/>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>868</v>
+        <v>853</v>
       </c>
       <c r="B258" t="s">
-        <v>869</v>
+        <v>854</v>
       </c>
       <c r="C258" t="s">
-        <v>869</v>
+        <v>854</v>
       </c>
       <c r="D258" t="s">
-        <v>26</v>
+        <v>887</v>
       </c>
       <c r="E258" t="s">
         <v>11</v>
@@ -10145,22 +9924,21 @@
         <v>609</v>
       </c>
       <c r="H258" s="1">
-        <v>45083</v>
-      </c>
-      <c r="I258"/>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>871</v>
+        <v>856</v>
       </c>
       <c r="B259" t="s">
-        <v>872</v>
+        <v>857</v>
       </c>
       <c r="C259" t="s">
-        <v>873</v>
+        <v>858</v>
       </c>
       <c r="D259" t="s">
-        <v>867</v>
+        <v>852</v>
       </c>
       <c r="E259" t="s">
         <v>23</v>
@@ -10174,20 +9952,19 @@
       <c r="H259" s="1">
         <v>45120</v>
       </c>
-      <c r="I259"/>
-    </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>874</v>
+        <v>859</v>
       </c>
       <c r="B260" t="s">
-        <v>875</v>
+        <v>860</v>
       </c>
       <c r="C260" t="s">
-        <v>879</v>
+        <v>914</v>
       </c>
       <c r="D260" t="s">
-        <v>876</v>
+        <v>861</v>
       </c>
       <c r="E260" t="s">
         <v>23</v>
@@ -10201,20 +9978,19 @@
       <c r="H260" s="1">
         <v>45132</v>
       </c>
-      <c r="I260"/>
-    </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>877</v>
+        <v>862</v>
       </c>
       <c r="B261" t="s">
-        <v>878</v>
+        <v>863</v>
       </c>
       <c r="C261" t="s">
-        <v>880</v>
+        <v>915</v>
       </c>
       <c r="D261" t="s">
-        <v>876</v>
+        <v>861</v>
       </c>
       <c r="E261" t="s">
         <v>23</v>
@@ -10228,20 +10004,19 @@
       <c r="H261" s="1">
         <v>45147</v>
       </c>
-      <c r="I261"/>
-    </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
       <c r="B262" t="s">
-        <v>882</v>
+        <v>865</v>
       </c>
       <c r="C262" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="D262" t="s">
-        <v>884</v>
+        <v>867</v>
       </c>
       <c r="E262" t="s">
         <v>23</v>
@@ -10255,20 +10030,19 @@
       <c r="H262" s="1">
         <v>45170</v>
       </c>
-      <c r="I262"/>
-    </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>885</v>
+        <v>868</v>
       </c>
       <c r="B263" t="s">
-        <v>886</v>
+        <v>869</v>
       </c>
       <c r="C263" t="s">
-        <v>887</v>
+        <v>870</v>
       </c>
       <c r="D263" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="E263" t="s">
         <v>23</v>
@@ -10282,20 +10056,19 @@
       <c r="H263" s="1">
         <v>45182</v>
       </c>
-      <c r="I263"/>
-    </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>889</v>
+        <v>872</v>
       </c>
       <c r="B264" t="s">
-        <v>890</v>
+        <v>873</v>
       </c>
       <c r="C264" t="s">
-        <v>891</v>
+        <v>874</v>
       </c>
       <c r="D264" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="E264" t="s">
         <v>23</v>
@@ -10309,20 +10082,19 @@
       <c r="H264" s="1">
         <v>45182</v>
       </c>
-      <c r="I264"/>
-    </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>893</v>
+        <v>876</v>
       </c>
       <c r="B265" t="s">
-        <v>894</v>
+        <v>877</v>
       </c>
       <c r="C265" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="D265" t="s">
-        <v>896</v>
+        <v>879</v>
       </c>
       <c r="E265" t="s">
         <v>23</v>
@@ -10336,20 +10108,19 @@
       <c r="H265" s="1">
         <v>45182</v>
       </c>
-      <c r="I265"/>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>897</v>
+        <v>880</v>
       </c>
       <c r="B266" t="s">
-        <v>898</v>
+        <v>881</v>
       </c>
       <c r="C266" t="s">
         <v>746</v>
       </c>
       <c r="D266" t="s">
-        <v>899</v>
+        <v>882</v>
       </c>
       <c r="E266" t="s">
         <v>23</v>
@@ -10363,20 +10134,19 @@
       <c r="H266" s="1">
         <v>45182</v>
       </c>
-      <c r="I266"/>
-    </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>900</v>
+        <v>883</v>
       </c>
       <c r="B267" t="s">
-        <v>901</v>
+        <v>884</v>
       </c>
       <c r="C267" t="s">
-        <v>902</v>
+        <v>885</v>
       </c>
       <c r="D267" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
       <c r="E267" t="s">
         <v>23</v>
@@ -10390,23 +10160,22 @@
       <c r="H267" s="1">
         <v>45182</v>
       </c>
-      <c r="I267"/>
-    </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>812</v>
+        <v>888</v>
       </c>
       <c r="B268" t="s">
-        <v>813</v>
+        <v>889</v>
       </c>
       <c r="C268" t="s">
-        <v>814</v>
+        <v>890</v>
       </c>
       <c r="D268" t="s">
-        <v>862</v>
+        <v>891</v>
       </c>
       <c r="E268" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F268">
         <v>290</v>
@@ -10415,9 +10184,86 @@
         <v>609</v>
       </c>
       <c r="H268" s="1">
-        <v>45034</v>
-      </c>
-      <c r="I268"/>
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>892</v>
+      </c>
+      <c r="B269" t="s">
+        <v>893</v>
+      </c>
+      <c r="C269" t="s">
+        <v>893</v>
+      </c>
+      <c r="D269" t="s">
+        <v>894</v>
+      </c>
+      <c r="E269" t="s">
+        <v>11</v>
+      </c>
+      <c r="F269">
+        <v>291</v>
+      </c>
+      <c r="G269" t="s">
+        <v>609</v>
+      </c>
+      <c r="H269" s="1">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>803</v>
+      </c>
+      <c r="B270" t="s">
+        <v>804</v>
+      </c>
+      <c r="C270" t="s">
+        <v>805</v>
+      </c>
+      <c r="D270" t="s">
+        <v>909</v>
+      </c>
+      <c r="E270" t="s">
+        <v>11</v>
+      </c>
+      <c r="F270">
+        <v>292</v>
+      </c>
+      <c r="G270" t="s">
+        <v>609</v>
+      </c>
+      <c r="H270" s="1">
+        <v>45225</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>910</v>
+      </c>
+      <c r="B271" t="s">
+        <v>911</v>
+      </c>
+      <c r="C271" t="s">
+        <v>912</v>
+      </c>
+      <c r="D271" t="s">
+        <v>913</v>
+      </c>
+      <c r="E271" t="s">
+        <v>23</v>
+      </c>
+      <c r="F271">
+        <v>293</v>
+      </c>
+      <c r="G271" t="s">
+        <v>609</v>
+      </c>
+      <c r="H271" s="1">
+        <v>45232</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improve loading time by loading short test plans and allowing to archive testplans
</commit_message>
<xml_diff>
--- a/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
+++ b/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/ske5_cdc_gov/Documents/+My_Documents/Shilpa/CPT/downloads/New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="588" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA720D03-471C-4BB3-8D10-EED2ED08E9F9}"/>
+  <xr:revisionPtr revIDLastSave="613" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{858CFE21-17AB-4EE1-9D61-B22B3715C80D}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="444" windowWidth="21252" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1788" yWindow="936" windowWidth="21252" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_cvx" sheetId="68" r:id="rId1"/>
+    <sheet name="Web_cvx" sheetId="69" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" localSheetId="0" hidden="1">Web_cvx!$A$1:$H$273</definedName>
+    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" localSheetId="0" hidden="1">Web_cvx!$A$1:$H$274</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -24,14 +24,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{6504600D-7A5F-4081-9D0B-AC21A5046F78}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes11111111111111111111111111111111111111111111111" type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{CA5EB419-6394-40E2-B334-5262DF4CED34}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes111111111111111111111111111111111111111111111111" type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;User ID=insidenipdbo;Initial Catalog=NIP_INSIDENIP;Data Source=DSDV-INFC-1601\qsrv1;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=D314248;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;NIP_INSIDENIP&quot;.&quot;dbo&quot;.&quot;tblCVXCodes&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="926">
   <si>
     <t>CVX Code</t>
   </si>
@@ -1791,33 +1791,15 @@
     <t>37</t>
   </si>
   <si>
-    <t>yellow fever</t>
-  </si>
-  <si>
-    <t>yellow fever vaccine</t>
-  </si>
-  <si>
     <t>This is the YF vaccine that has been available in the US for years. It is stabilized with sorbitol and gelatin.</t>
   </si>
   <si>
     <t>183</t>
   </si>
   <si>
-    <t>Yellow fever vaccine - alt</t>
-  </si>
-  <si>
-    <t>Yellow fever vaccine alternative formulation</t>
-  </si>
-  <si>
-    <t>This vaccine is stabilized with sorbitol and lactose and has been used outside the US for some time. It will be made available in the US.</t>
-  </si>
-  <si>
     <t>184</t>
   </si>
   <si>
-    <t>Yellow fever, unspecified formulation</t>
-  </si>
-  <si>
     <t>Yellow fever vaccine, unspecified formulation</t>
   </si>
   <si>
@@ -2800,6 +2782,33 @@
   </si>
   <si>
     <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ, (nirsevimab-alip), 1 mL, neonates and children to 24 months</t>
+  </si>
+  <si>
+    <t>yellow fever live</t>
+  </si>
+  <si>
+    <t>yellow fever vaccine live</t>
+  </si>
+  <si>
+    <t>Yellow fever vaccine live - alt</t>
+  </si>
+  <si>
+    <t>Yellow fever vaccine live - alternative formulation for vaccine shortage</t>
+  </si>
+  <si>
+    <t>This CVX is associated to an FDA unapproved drug to be used when there is a drug shortage. Stabilized with sorbitol and lactose and has been used outside the US for some time.</t>
+  </si>
+  <si>
+    <t>Yellow fever, unspecified</t>
+  </si>
+  <si>
+    <t>319</t>
+  </si>
+  <si>
+    <t>Anthrax vaccine, unspecified</t>
+  </si>
+  <si>
+    <t>Unspecified code to record historic administration when specific product is unknown</t>
   </si>
 </sst>
 </file>
@@ -2863,7 +2872,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes" connectionId="1" xr16:uid="{A5BDA0E7-6107-4A65-B0AE-77D317BEC162}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" connectionId="1" xr16:uid="{D02DEEDB-31D5-426C-B588-3043BA303275}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="11">
     <queryTableFields count="8">
       <queryTableField id="2" name="cvx_code" tableColumnId="2"/>
@@ -2883,16 +2892,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4227F0BB-1E04-4A56-8010-DCB5E7510EFC}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" ref="A1:H273" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8622DAB5-78D5-4996-AC2A-9BE56E619D7D}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" ref="A1:H274" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{45364DD6-CDD1-4289-B07F-5499C77575C1}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{B1E37F9F-03F7-49DE-B415-FB09DAB8C5E6}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{C6FD4DF8-2FA3-45F2-86F6-2BBD76618FFD}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{FD72A10A-855D-4437-8315-3E7C5BD51AAD}" uniqueName="5" name="Note" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{71AE3AF8-BF3E-4885-B700-73DDA500E7D2}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
-    <tableColumn id="1" xr3:uid="{E096AF81-BD99-4BBF-980A-FF0B3F04900B}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
-    <tableColumn id="8" xr3:uid="{D46DC246-6A6E-4C5A-83F8-CB51543CD8DF}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{AE74171D-8627-41A4-930E-F8D96919F1F9}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{2118B836-FCDC-4A04-B87E-E7774FE5052F}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{43D3AD75-8247-4AF4-836B-71EAE5205EF2}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{36A88CFA-E5B9-4FA6-91E8-1F24120E6696}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{D5413BAC-05D2-4D3A-86B6-312F6D0D7553}" uniqueName="5" name="Note" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{D4171E85-8D94-4A78-8590-12718C519E96}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{6401A5D1-6B09-4DF8-B63C-022C5BCE0E8A}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
+    <tableColumn id="8" xr3:uid="{CD46FD17-F8D9-4E32-B252-2192943CD905}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{A75629BE-D845-4E9D-AA23-47E8394504D4}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3184,24 +3193,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57439980-945F-4441-8EB4-7690A6B4EF0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB9EA7B-2066-4D27-BF4A-F4B3F6B47552}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H273"/>
+  <dimension ref="A1:H274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="C260" sqref="C260"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="3" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3233,7 +3243,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -3251,7 +3261,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H2" s="1">
         <v>40326</v>
@@ -3277,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H3" s="1">
         <v>40326</v>
@@ -3303,7 +3313,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H4" s="1">
         <v>40451</v>
@@ -3314,10 +3324,10 @@
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="C5" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="D5" t="s">
         <v>26</v>
@@ -3329,7 +3339,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H5" s="1">
         <v>45316</v>
@@ -3355,7 +3365,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H6" s="1">
         <v>40326</v>
@@ -3381,7 +3391,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H7" s="1">
         <v>44078</v>
@@ -3407,7 +3417,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H8" s="1">
         <v>42538</v>
@@ -3433,7 +3443,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H9" s="1">
         <v>44078</v>
@@ -3444,13 +3454,13 @@
         <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="C10" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="D10" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -3459,7 +3469,7 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H10" s="1">
         <v>44973</v>
@@ -3485,7 +3495,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H11" s="1">
         <v>44078</v>
@@ -3511,7 +3521,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H12" s="1">
         <v>40326</v>
@@ -3537,7 +3547,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H13" s="1">
         <v>40326</v>
@@ -3563,7 +3573,7 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H14" s="1">
         <v>40326</v>
@@ -3589,7 +3599,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H15" s="1">
         <v>40451</v>
@@ -3615,7 +3625,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H16" s="1">
         <v>40326</v>
@@ -3641,7 +3651,7 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H17" s="1">
         <v>42814</v>
@@ -3667,7 +3677,7 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H18" s="1">
         <v>40326</v>
@@ -3693,7 +3703,7 @@
         <v>19</v>
       </c>
       <c r="G19" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H19" s="1">
         <v>40326</v>
@@ -3719,7 +3729,7 @@
         <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H20" s="1">
         <v>40326</v>
@@ -3745,7 +3755,7 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H21" s="1">
         <v>42817</v>
@@ -3771,7 +3781,7 @@
         <v>23</v>
       </c>
       <c r="G22" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H22" s="1">
         <v>42510</v>
@@ -3797,7 +3807,7 @@
         <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H23" s="1">
         <v>44083</v>
@@ -3823,7 +3833,7 @@
         <v>25</v>
       </c>
       <c r="G24" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H24" s="1">
         <v>40326</v>
@@ -3849,7 +3859,7 @@
         <v>26</v>
       </c>
       <c r="G25" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H25" s="1">
         <v>40326</v>
@@ -3875,7 +3885,7 @@
         <v>27</v>
       </c>
       <c r="G26" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H26" s="1">
         <v>40326</v>
@@ -3901,7 +3911,7 @@
         <v>28</v>
       </c>
       <c r="G27" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H27" s="1">
         <v>40451</v>
@@ -3927,7 +3937,7 @@
         <v>29</v>
       </c>
       <c r="G28" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H28" s="1">
         <v>40451</v>
@@ -3953,7 +3963,7 @@
         <v>30</v>
       </c>
       <c r="G29" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H29" s="1">
         <v>40326</v>
@@ -3979,7 +3989,7 @@
         <v>31</v>
       </c>
       <c r="G30" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H30" s="1">
         <v>44078</v>
@@ -3996,7 +4006,7 @@
         <v>145</v>
       </c>
       <c r="D31" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
@@ -4005,7 +4015,7 @@
         <v>32</v>
       </c>
       <c r="G31" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H31" s="1">
         <v>43230</v>
@@ -4031,7 +4041,7 @@
         <v>33</v>
       </c>
       <c r="G32" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H32" s="1">
         <v>40326</v>
@@ -4048,7 +4058,7 @@
         <v>152</v>
       </c>
       <c r="D33" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="E33" t="s">
         <v>23</v>
@@ -4057,7 +4067,7 @@
         <v>34</v>
       </c>
       <c r="G33" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H33" s="1">
         <v>43230</v>
@@ -4074,7 +4084,7 @@
         <v>155</v>
       </c>
       <c r="D34" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="E34" t="s">
         <v>23</v>
@@ -4083,7 +4093,7 @@
         <v>35</v>
       </c>
       <c r="G34" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H34" s="1">
         <v>43593</v>
@@ -4109,7 +4119,7 @@
         <v>36</v>
       </c>
       <c r="G35" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H35" s="1">
         <v>40451</v>
@@ -4135,7 +4145,7 @@
         <v>37</v>
       </c>
       <c r="G36" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H36" s="1">
         <v>44083</v>
@@ -4161,7 +4171,7 @@
         <v>38</v>
       </c>
       <c r="G37" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H37" s="1">
         <v>44083</v>
@@ -4187,7 +4197,7 @@
         <v>39</v>
       </c>
       <c r="G38" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H38" s="1">
         <v>44083</v>
@@ -4213,7 +4223,7 @@
         <v>40</v>
       </c>
       <c r="G39" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H39" s="1">
         <v>40326</v>
@@ -4239,7 +4249,7 @@
         <v>41</v>
       </c>
       <c r="G40" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H40" s="1">
         <v>40326</v>
@@ -4265,7 +4275,7 @@
         <v>42</v>
       </c>
       <c r="G41" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H41" s="1">
         <v>40326</v>
@@ -4291,7 +4301,7 @@
         <v>43</v>
       </c>
       <c r="G42" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H42" s="1">
         <v>40326</v>
@@ -4317,7 +4327,7 @@
         <v>44</v>
       </c>
       <c r="G43" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H43" s="1">
         <v>40451</v>
@@ -4343,7 +4353,7 @@
         <v>45</v>
       </c>
       <c r="G44" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H44" s="1">
         <v>42440</v>
@@ -4369,7 +4379,7 @@
         <v>46</v>
       </c>
       <c r="G45" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H45" s="1">
         <v>44083</v>
@@ -4395,7 +4405,7 @@
         <v>47</v>
       </c>
       <c r="G46" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H46" s="1">
         <v>40326</v>
@@ -4421,7 +4431,7 @@
         <v>49</v>
       </c>
       <c r="G47" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H47" s="1">
         <v>43984</v>
@@ -4447,7 +4457,7 @@
         <v>51</v>
       </c>
       <c r="G48" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H48" s="1">
         <v>44078</v>
@@ -4473,7 +4483,7 @@
         <v>52</v>
       </c>
       <c r="G49" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H49" s="1">
         <v>44078</v>
@@ -4499,7 +4509,7 @@
         <v>53</v>
       </c>
       <c r="G50" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H50" s="1">
         <v>44994</v>
@@ -4525,7 +4535,7 @@
         <v>54</v>
       </c>
       <c r="G51" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H51" s="1">
         <v>41904</v>
@@ -4551,7 +4561,7 @@
         <v>55</v>
       </c>
       <c r="G52" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H52" s="1">
         <v>40451</v>
@@ -4577,7 +4587,7 @@
         <v>56</v>
       </c>
       <c r="G53" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H53" s="1">
         <v>40326</v>
@@ -4603,7 +4613,7 @@
         <v>57</v>
       </c>
       <c r="G54" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H54" s="1">
         <v>40451</v>
@@ -4629,7 +4639,7 @@
         <v>58</v>
       </c>
       <c r="G55" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H55" s="1">
         <v>40326</v>
@@ -4655,7 +4665,7 @@
         <v>60</v>
       </c>
       <c r="G56" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H56" s="1">
         <v>40326</v>
@@ -4681,7 +4691,7 @@
         <v>61</v>
       </c>
       <c r="G57" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H57" s="1">
         <v>42776</v>
@@ -4707,7 +4717,7 @@
         <v>62</v>
       </c>
       <c r="G58" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H58" s="1">
         <v>40451</v>
@@ -4733,7 +4743,7 @@
         <v>63</v>
       </c>
       <c r="G59" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H59" s="1">
         <v>42271</v>
@@ -4759,7 +4769,7 @@
         <v>64</v>
       </c>
       <c r="G60" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H60" s="1">
         <v>44083</v>
@@ -4785,7 +4795,7 @@
         <v>65</v>
       </c>
       <c r="G61" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H61" s="1">
         <v>44083</v>
@@ -4811,7 +4821,7 @@
         <v>66</v>
       </c>
       <c r="G62" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H62" s="1">
         <v>44083</v>
@@ -4837,7 +4847,7 @@
         <v>67</v>
       </c>
       <c r="G63" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H63" s="1">
         <v>40326</v>
@@ -4863,7 +4873,7 @@
         <v>68</v>
       </c>
       <c r="G64" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H64" s="1">
         <v>40326</v>
@@ -4889,7 +4899,7 @@
         <v>69</v>
       </c>
       <c r="G65" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H65" s="1">
         <v>40326</v>
@@ -4915,7 +4925,7 @@
         <v>70</v>
       </c>
       <c r="G66" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H66" s="1">
         <v>40326</v>
@@ -4941,7 +4951,7 @@
         <v>71</v>
       </c>
       <c r="G67" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H67" s="1">
         <v>44083</v>
@@ -4967,7 +4977,7 @@
         <v>72</v>
       </c>
       <c r="G68" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H68" s="1">
         <v>40421</v>
@@ -4993,7 +5003,7 @@
         <v>73</v>
       </c>
       <c r="G69" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H69" s="1">
         <v>44083</v>
@@ -5019,7 +5029,7 @@
         <v>74</v>
       </c>
       <c r="G70" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H70" s="1">
         <v>43035</v>
@@ -5045,7 +5055,7 @@
         <v>75</v>
       </c>
       <c r="G71" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H71" s="1">
         <v>40326</v>
@@ -5071,7 +5081,7 @@
         <v>76</v>
       </c>
       <c r="G72" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H72" s="1">
         <v>40326</v>
@@ -5097,7 +5107,7 @@
         <v>77</v>
       </c>
       <c r="G73" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H73" s="1">
         <v>42339</v>
@@ -5123,7 +5133,7 @@
         <v>79</v>
       </c>
       <c r="G74" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H74" s="1">
         <v>42173</v>
@@ -5149,7 +5159,7 @@
         <v>80</v>
       </c>
       <c r="G75" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H75" s="1">
         <v>40326</v>
@@ -5175,7 +5185,7 @@
         <v>81</v>
       </c>
       <c r="G76" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H76" s="1">
         <v>40326</v>
@@ -5201,7 +5211,7 @@
         <v>82</v>
       </c>
       <c r="G77" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H77" s="1">
         <v>43237</v>
@@ -5227,7 +5237,7 @@
         <v>83</v>
       </c>
       <c r="G78" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H78" s="1">
         <v>40326</v>
@@ -5253,7 +5263,7 @@
         <v>84</v>
       </c>
       <c r="G79" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H79" s="1">
         <v>41816</v>
@@ -5279,7 +5289,7 @@
         <v>85</v>
       </c>
       <c r="G80" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H80" s="1">
         <v>40451</v>
@@ -5305,7 +5315,7 @@
         <v>86</v>
       </c>
       <c r="G81" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H81" s="1">
         <v>44083</v>
@@ -5331,7 +5341,7 @@
         <v>87</v>
       </c>
       <c r="G82" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H82" s="1">
         <v>42661</v>
@@ -5357,7 +5367,7 @@
         <v>88</v>
       </c>
       <c r="G83" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H83" s="1">
         <v>42173</v>
@@ -5383,7 +5393,7 @@
         <v>89</v>
       </c>
       <c r="G84" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H84" s="1">
         <v>40451</v>
@@ -5409,7 +5419,7 @@
         <v>90</v>
       </c>
       <c r="G85" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H85" s="1">
         <v>44083</v>
@@ -5435,7 +5445,7 @@
         <v>91</v>
       </c>
       <c r="G86" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H86" s="1">
         <v>44083</v>
@@ -5461,7 +5471,7 @@
         <v>92</v>
       </c>
       <c r="G87" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H87" s="1">
         <v>44078</v>
@@ -5487,7 +5497,7 @@
         <v>93</v>
       </c>
       <c r="G88" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H88" s="1">
         <v>40326</v>
@@ -5513,7 +5523,7 @@
         <v>95</v>
       </c>
       <c r="G89" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H89" s="1">
         <v>40451</v>
@@ -5539,7 +5549,7 @@
         <v>97</v>
       </c>
       <c r="G90" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H90" s="1">
         <v>40326</v>
@@ -5565,7 +5575,7 @@
         <v>99</v>
       </c>
       <c r="G91" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H91" s="1">
         <v>40326</v>
@@ -5582,7 +5592,7 @@
         <v>481</v>
       </c>
       <c r="D92" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -5591,7 +5601,7 @@
         <v>101</v>
       </c>
       <c r="G92" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H92" s="1">
         <v>45126</v>
@@ -5617,7 +5627,7 @@
         <v>102</v>
       </c>
       <c r="G93" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H93" s="1">
         <v>44078</v>
@@ -5643,7 +5653,7 @@
         <v>103</v>
       </c>
       <c r="G94" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H94" s="1">
         <v>42173</v>
@@ -5669,7 +5679,7 @@
         <v>104</v>
       </c>
       <c r="G95" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H95" s="1">
         <v>40326</v>
@@ -5695,7 +5705,7 @@
         <v>105</v>
       </c>
       <c r="G96" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H96" s="1">
         <v>44994</v>
@@ -5721,7 +5731,7 @@
         <v>106</v>
       </c>
       <c r="G97" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H97" s="1">
         <v>45316</v>
@@ -5747,7 +5757,7 @@
         <v>107</v>
       </c>
       <c r="G98" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H98" s="1">
         <v>43035</v>
@@ -5773,7 +5783,7 @@
         <v>108</v>
       </c>
       <c r="G99" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H99" s="1">
         <v>40326</v>
@@ -5799,7 +5809,7 @@
         <v>110</v>
       </c>
       <c r="G100" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H100" s="1">
         <v>42230</v>
@@ -5825,7 +5835,7 @@
         <v>111</v>
       </c>
       <c r="G101" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H101" s="1">
         <v>40451</v>
@@ -5836,13 +5846,13 @@
         <v>521</v>
       </c>
       <c r="B102" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="C102" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="D102" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="E102" t="s">
         <v>47</v>
@@ -5851,7 +5861,7 @@
         <v>112</v>
       </c>
       <c r="G102" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H102" s="1">
         <v>44624</v>
@@ -5877,7 +5887,7 @@
         <v>113</v>
       </c>
       <c r="G103" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H103" s="1">
         <v>44078</v>
@@ -5903,7 +5913,7 @@
         <v>114</v>
       </c>
       <c r="G104" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H104" s="1">
         <v>44994</v>
@@ -5929,7 +5939,7 @@
         <v>115</v>
       </c>
       <c r="G105" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H105" s="1">
         <v>44994</v>
@@ -5955,7 +5965,7 @@
         <v>116</v>
       </c>
       <c r="G106" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H106" s="1">
         <v>44994</v>
@@ -5981,7 +5991,7 @@
         <v>117</v>
       </c>
       <c r="G107" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H107" s="1">
         <v>44994</v>
@@ -6007,7 +6017,7 @@
         <v>118</v>
       </c>
       <c r="G108" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H108" s="1">
         <v>40326</v>
@@ -6033,7 +6043,7 @@
         <v>119</v>
       </c>
       <c r="G109" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H109" s="1">
         <v>40451</v>
@@ -6059,7 +6069,7 @@
         <v>120</v>
       </c>
       <c r="G110" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H110" s="1">
         <v>40326</v>
@@ -6085,7 +6095,7 @@
         <v>121</v>
       </c>
       <c r="G111" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H111" s="1">
         <v>42229</v>
@@ -6111,7 +6121,7 @@
         <v>122</v>
       </c>
       <c r="G112" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H112" s="1">
         <v>42173</v>
@@ -6137,7 +6147,7 @@
         <v>123</v>
       </c>
       <c r="G113" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H113" s="1">
         <v>40326</v>
@@ -6163,7 +6173,7 @@
         <v>124</v>
       </c>
       <c r="G114" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H114" s="1">
         <v>40326</v>
@@ -6189,7 +6199,7 @@
         <v>125</v>
       </c>
       <c r="G115" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H115" s="1">
         <v>40326</v>
@@ -6215,7 +6225,7 @@
         <v>126</v>
       </c>
       <c r="G116" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H116" s="1">
         <v>44078</v>
@@ -6241,7 +6251,7 @@
         <v>127</v>
       </c>
       <c r="G117" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H117" s="1">
         <v>40326</v>
@@ -6267,7 +6277,7 @@
         <v>128</v>
       </c>
       <c r="G118" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H118" s="1">
         <v>40326</v>
@@ -6293,7 +6303,7 @@
         <v>129</v>
       </c>
       <c r="G119" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H119" s="1">
         <v>40326</v>
@@ -6319,7 +6329,7 @@
         <v>130</v>
       </c>
       <c r="G120" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H120" s="1">
         <v>40451</v>
@@ -6345,7 +6355,7 @@
         <v>131</v>
       </c>
       <c r="G121" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H121" s="1">
         <v>44078</v>
@@ -6371,7 +6381,7 @@
         <v>132</v>
       </c>
       <c r="G122" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H122" s="1">
         <v>44083</v>
@@ -6382,13 +6392,13 @@
         <v>585</v>
       </c>
       <c r="B123" t="s">
+        <v>917</v>
+      </c>
+      <c r="C123" t="s">
+        <v>918</v>
+      </c>
+      <c r="D123" t="s">
         <v>586</v>
-      </c>
-      <c r="C123" t="s">
-        <v>587</v>
-      </c>
-      <c r="D123" t="s">
-        <v>588</v>
       </c>
       <c r="E123" t="s">
         <v>23</v>
@@ -6397,21 +6407,21 @@
         <v>134</v>
       </c>
       <c r="G123" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H123" s="1">
-        <v>42796</v>
+        <v>45358</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B124" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="C124" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="D124" t="s">
         <v>26</v>
@@ -6423,7 +6433,7 @@
         <v>135</v>
       </c>
       <c r="G124" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H124" s="1">
         <v>40326</v>
@@ -6449,7 +6459,7 @@
         <v>137</v>
       </c>
       <c r="G125" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H125" s="1">
         <v>44994</v>
@@ -6475,7 +6485,7 @@
         <v>138</v>
       </c>
       <c r="G126" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H126" s="1">
         <v>44131</v>
@@ -6501,7 +6511,7 @@
         <v>139</v>
       </c>
       <c r="G127" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H127" s="1">
         <v>44083</v>
@@ -6527,7 +6537,7 @@
         <v>141</v>
       </c>
       <c r="G128" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H128" s="1">
         <v>40326</v>
@@ -6553,7 +6563,7 @@
         <v>142</v>
       </c>
       <c r="G129" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H129" s="1">
         <v>40326</v>
@@ -6579,7 +6589,7 @@
         <v>144</v>
       </c>
       <c r="G130" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H130" s="1">
         <v>40451</v>
@@ -6605,7 +6615,7 @@
         <v>145</v>
       </c>
       <c r="G131" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H131" s="1">
         <v>40326</v>
@@ -6631,7 +6641,7 @@
         <v>146</v>
       </c>
       <c r="G132" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H132" s="1">
         <v>40326</v>
@@ -6657,7 +6667,7 @@
         <v>147</v>
       </c>
       <c r="G133" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H133" s="1">
         <v>40326</v>
@@ -6671,7 +6681,7 @@
         <v>95</v>
       </c>
       <c r="C134" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="D134" t="s">
         <v>96</v>
@@ -6683,7 +6693,7 @@
         <v>148</v>
       </c>
       <c r="G134" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H134" s="1">
         <v>43230</v>
@@ -6709,7 +6719,7 @@
         <v>149</v>
       </c>
       <c r="G135" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H135" s="1">
         <v>40418</v>
@@ -6735,7 +6745,7 @@
         <v>150</v>
       </c>
       <c r="G136" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H136" s="1">
         <v>40418</v>
@@ -6761,7 +6771,7 @@
         <v>151</v>
       </c>
       <c r="G137" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H137" s="1">
         <v>40418</v>
@@ -6787,7 +6797,7 @@
         <v>152</v>
       </c>
       <c r="G138" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H138" s="1">
         <v>40418</v>
@@ -6813,7 +6823,7 @@
         <v>154</v>
       </c>
       <c r="G139" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H139" s="1">
         <v>40451</v>
@@ -6830,7 +6840,7 @@
         <v>508</v>
       </c>
       <c r="D140" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="E140" t="s">
         <v>11</v>
@@ -6839,7 +6849,7 @@
         <v>155</v>
       </c>
       <c r="G140" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H140" s="1">
         <v>43704</v>
@@ -6856,7 +6866,7 @@
         <v>265</v>
       </c>
       <c r="D141" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="E141" t="s">
         <v>11</v>
@@ -6865,7 +6875,7 @@
         <v>156</v>
       </c>
       <c r="G141" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H141" s="1">
         <v>44910</v>
@@ -6891,7 +6901,7 @@
         <v>157</v>
       </c>
       <c r="G142" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H142" s="1">
         <v>40451</v>
@@ -6917,7 +6927,7 @@
         <v>159</v>
       </c>
       <c r="G143" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H143" s="1">
         <v>41472</v>
@@ -6943,7 +6953,7 @@
         <v>160</v>
       </c>
       <c r="G144" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H144" s="1">
         <v>42230</v>
@@ -6969,7 +6979,7 @@
         <v>161</v>
       </c>
       <c r="G145" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H145" s="1">
         <v>40622</v>
@@ -6986,7 +6996,7 @@
         <v>268</v>
       </c>
       <c r="D146" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="E146" t="s">
         <v>11</v>
@@ -6995,7 +7005,7 @@
         <v>162</v>
       </c>
       <c r="G146" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H146" s="1">
         <v>44910</v>
@@ -7021,7 +7031,7 @@
         <v>163</v>
       </c>
       <c r="G147" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H147" s="1">
         <v>44083</v>
@@ -7038,7 +7048,7 @@
         <v>77</v>
       </c>
       <c r="D148" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="E148" t="s">
         <v>23</v>
@@ -7047,7 +7057,7 @@
         <v>164</v>
       </c>
       <c r="G148" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H148" s="1">
         <v>44783</v>
@@ -7073,7 +7083,7 @@
         <v>165</v>
       </c>
       <c r="G149" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H149" s="1">
         <v>40947</v>
@@ -7099,7 +7109,7 @@
         <v>166</v>
       </c>
       <c r="G150" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H150" s="1">
         <v>43231</v>
@@ -7125,7 +7135,7 @@
         <v>167</v>
       </c>
       <c r="G151" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H151" s="1">
         <v>41472</v>
@@ -7151,7 +7161,7 @@
         <v>168</v>
       </c>
       <c r="G152" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H152" s="1">
         <v>41472</v>
@@ -7177,7 +7187,7 @@
         <v>169</v>
       </c>
       <c r="G153" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H153" s="1">
         <v>41302</v>
@@ -7203,7 +7213,7 @@
         <v>170</v>
       </c>
       <c r="G154" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H154" s="1">
         <v>41302</v>
@@ -7229,7 +7239,7 @@
         <v>171</v>
       </c>
       <c r="G155" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H155" s="1">
         <v>42545</v>
@@ -7255,7 +7265,7 @@
         <v>172</v>
       </c>
       <c r="G156" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H156" s="1">
         <v>44083</v>
@@ -7281,7 +7291,7 @@
         <v>173</v>
       </c>
       <c r="G157" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H157" s="1">
         <v>41472</v>
@@ -7307,7 +7317,7 @@
         <v>174</v>
       </c>
       <c r="G158" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H158" s="1">
         <v>44078</v>
@@ -7333,7 +7343,7 @@
         <v>175</v>
       </c>
       <c r="G159" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H159" s="1">
         <v>44078</v>
@@ -7359,7 +7369,7 @@
         <v>176</v>
       </c>
       <c r="G160" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H160" s="1">
         <v>41506</v>
@@ -7385,7 +7395,7 @@
         <v>177</v>
       </c>
       <c r="G161" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H161" s="1">
         <v>44994</v>
@@ -7411,7 +7421,7 @@
         <v>178</v>
       </c>
       <c r="G162" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H162" s="1">
         <v>41786</v>
@@ -7437,7 +7447,7 @@
         <v>179</v>
       </c>
       <c r="G163" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H163" s="1">
         <v>44131</v>
@@ -7463,7 +7473,7 @@
         <v>180</v>
       </c>
       <c r="G164" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H164" s="1">
         <v>41843</v>
@@ -7489,7 +7499,7 @@
         <v>181</v>
       </c>
       <c r="G165" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H165" s="1">
         <v>41946</v>
@@ -7515,7 +7525,7 @@
         <v>182</v>
       </c>
       <c r="G166" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H166" s="1">
         <v>42037</v>
@@ -7541,7 +7551,7 @@
         <v>183</v>
       </c>
       <c r="G167" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H167" s="1">
         <v>41946</v>
@@ -7567,7 +7577,7 @@
         <v>184</v>
       </c>
       <c r="G168" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H168" s="1">
         <v>41984</v>
@@ -7584,7 +7594,7 @@
         <v>246</v>
       </c>
       <c r="D169" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="E169" t="s">
         <v>11</v>
@@ -7593,7 +7603,7 @@
         <v>185</v>
       </c>
       <c r="G169" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H169" s="1">
         <v>44910</v>
@@ -7619,7 +7629,7 @@
         <v>188</v>
       </c>
       <c r="G170" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H170" s="1">
         <v>42339</v>
@@ -7645,7 +7655,7 @@
         <v>189</v>
       </c>
       <c r="G171" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H171" s="1">
         <v>42348</v>
@@ -7671,7 +7681,7 @@
         <v>190</v>
       </c>
       <c r="G172" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H172" s="1">
         <v>42500</v>
@@ -7697,7 +7707,7 @@
         <v>191</v>
       </c>
       <c r="G173" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H173" s="1">
         <v>42510</v>
@@ -7723,7 +7733,7 @@
         <v>192</v>
       </c>
       <c r="G174" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H174" s="1">
         <v>45316</v>
@@ -7749,7 +7759,7 @@
         <v>193</v>
       </c>
       <c r="G175" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H175" s="1">
         <v>42538</v>
@@ -7775,7 +7785,7 @@
         <v>194</v>
       </c>
       <c r="G176" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H176" s="1">
         <v>42538</v>
@@ -7801,7 +7811,7 @@
         <v>195</v>
       </c>
       <c r="G177" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H177" s="1">
         <v>42538</v>
@@ -7827,7 +7837,7 @@
         <v>196</v>
       </c>
       <c r="G178" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H178" s="1">
         <v>42661</v>
@@ -7853,7 +7863,7 @@
         <v>197</v>
       </c>
       <c r="G179" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H179" s="1">
         <v>42661</v>
@@ -7879,7 +7889,7 @@
         <v>201</v>
       </c>
       <c r="G180" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H180" s="1">
         <v>42723</v>
@@ -7905,7 +7915,7 @@
         <v>202</v>
       </c>
       <c r="G181" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H181" s="1">
         <v>42752</v>
@@ -7931,7 +7941,7 @@
         <v>203</v>
       </c>
       <c r="G182" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H182" s="1">
         <v>42752</v>
@@ -7957,7 +7967,7 @@
         <v>204</v>
       </c>
       <c r="G183" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H183" s="1">
         <v>44083</v>
@@ -7983,7 +7993,7 @@
         <v>205</v>
       </c>
       <c r="G184" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="H184" s="1">
         <v>44078</v>
@@ -8009,7 +8019,7 @@
         <v>206</v>
       </c>
       <c r="G185" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H185" s="1">
         <v>42752</v>
@@ -8017,16 +8027,16 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B186" t="s">
-        <v>590</v>
+        <v>919</v>
       </c>
       <c r="C186" t="s">
-        <v>591</v>
+        <v>920</v>
       </c>
       <c r="D186" t="s">
-        <v>592</v>
+        <v>921</v>
       </c>
       <c r="E186" t="s">
         <v>23</v>
@@ -8035,21 +8045,21 @@
         <v>207</v>
       </c>
       <c r="G186" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H186" s="1">
-        <v>42796</v>
+        <v>45358</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="B187" t="s">
-        <v>594</v>
+        <v>922</v>
       </c>
       <c r="C187" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="D187" t="s">
         <v>26</v>
@@ -8061,10 +8071,10 @@
         <v>208</v>
       </c>
       <c r="G187" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H187" s="1">
-        <v>42796</v>
+        <v>45358</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
@@ -8087,7 +8097,7 @@
         <v>209</v>
       </c>
       <c r="G188" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H188" s="1">
         <v>42846</v>
@@ -8101,7 +8111,7 @@
         <v>233</v>
       </c>
       <c r="C189" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="D189" t="s">
         <v>26</v>
@@ -8113,7 +8123,7 @@
         <v>210</v>
       </c>
       <c r="G189" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H189" s="1">
         <v>45316</v>
@@ -8121,13 +8131,13 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="B190" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C190" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D190" t="s">
         <v>26</v>
@@ -8139,7 +8149,7 @@
         <v>211</v>
       </c>
       <c r="G190" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H190" s="1">
         <v>43035</v>
@@ -8147,16 +8157,16 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="B191" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="C191" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="D191" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="E191" t="s">
         <v>11</v>
@@ -8165,7 +8175,7 @@
         <v>212</v>
       </c>
       <c r="G191" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H191" s="1">
         <v>43035</v>
@@ -8176,10 +8186,10 @@
         <v>142</v>
       </c>
       <c r="B192" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="C192" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="D192" t="s">
         <v>26</v>
@@ -8191,7 +8201,7 @@
         <v>213</v>
       </c>
       <c r="G192" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H192" s="1">
         <v>43230</v>
@@ -8199,13 +8209,13 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B193" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="C193" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="D193" t="s">
         <v>26</v>
@@ -8217,7 +8227,7 @@
         <v>214</v>
       </c>
       <c r="G193" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H193" s="1">
         <v>44943</v>
@@ -8225,13 +8235,13 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B194" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="C194" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="D194" t="s">
         <v>26</v>
@@ -8243,7 +8253,7 @@
         <v>215</v>
       </c>
       <c r="G194" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H194" s="1">
         <v>43230</v>
@@ -8251,13 +8261,13 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B195" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="C195" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="D195" t="s">
         <v>26</v>
@@ -8269,7 +8279,7 @@
         <v>216</v>
       </c>
       <c r="G195" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H195" s="1">
         <v>43230</v>
@@ -8277,16 +8287,16 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B196" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="C196" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="D196" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="E196" t="s">
         <v>47</v>
@@ -8295,7 +8305,7 @@
         <v>217</v>
       </c>
       <c r="G196" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H196" s="1">
         <v>43333</v>
@@ -8303,16 +8313,16 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="B197" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="C197" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="D197" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="E197" t="s">
         <v>11</v>
@@ -8321,7 +8331,7 @@
         <v>218</v>
       </c>
       <c r="G197" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H197" s="1">
         <v>44028</v>
@@ -8329,16 +8339,16 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B198" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="C198" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="D198" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="E198" t="s">
         <v>47</v>
@@ -8347,7 +8357,7 @@
         <v>219</v>
       </c>
       <c r="G198" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H198" s="1">
         <v>44943</v>
@@ -8355,16 +8365,16 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="B199" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C199" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="D199" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="E199" t="s">
         <v>23</v>
@@ -8373,7 +8383,7 @@
         <v>220</v>
       </c>
       <c r="G199" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H199" s="1">
         <v>43692</v>
@@ -8381,16 +8391,16 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="B200" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="C200" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="D200" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="E200" t="s">
         <v>23</v>
@@ -8399,7 +8409,7 @@
         <v>221</v>
       </c>
       <c r="G200" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H200" s="1">
         <v>44943</v>
@@ -8407,16 +8417,16 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B201" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="C201" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="D201" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="E201" t="s">
         <v>23</v>
@@ -8425,7 +8435,7 @@
         <v>222</v>
       </c>
       <c r="G201" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H201" s="1">
         <v>44943</v>
@@ -8433,16 +8443,16 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="B202" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="C202" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="D202" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="E202" t="s">
         <v>23</v>
@@ -8451,7 +8461,7 @@
         <v>223</v>
       </c>
       <c r="G202" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H202" s="1">
         <v>44943</v>
@@ -8459,16 +8469,16 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="B203" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C203" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="D203" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="E203" t="s">
         <v>23</v>
@@ -8477,7 +8487,7 @@
         <v>224</v>
       </c>
       <c r="G203" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H203" s="1">
         <v>44943</v>
@@ -8485,16 +8495,16 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B204" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="C204" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="D204" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="E204" t="s">
         <v>47</v>
@@ -8503,7 +8513,7 @@
         <v>225</v>
       </c>
       <c r="G204" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H204" s="1">
         <v>44943</v>
@@ -8511,13 +8521,13 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B205" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="C205" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="D205" t="s">
         <v>26</v>
@@ -8529,7 +8539,7 @@
         <v>226</v>
       </c>
       <c r="G205" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H205" s="1">
         <v>44952</v>
@@ -8537,13 +8547,13 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B206" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="C206" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="D206" t="s">
         <v>26</v>
@@ -8555,7 +8565,7 @@
         <v>228</v>
       </c>
       <c r="G206" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H206" s="1">
         <v>44943</v>
@@ -8563,16 +8573,16 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="B207" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="C207" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="D207" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="E207" t="s">
         <v>23</v>
@@ -8581,7 +8591,7 @@
         <v>229</v>
       </c>
       <c r="G207" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H207" s="1">
         <v>44971</v>
@@ -8589,16 +8599,16 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B208" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="C208" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="D208" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="E208" t="s">
         <v>11</v>
@@ -8607,7 +8617,7 @@
         <v>230</v>
       </c>
       <c r="G208" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H208" s="1">
         <v>45223</v>
@@ -8615,16 +8625,16 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="B209" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="C209" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="D209" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="E209" t="s">
         <v>11</v>
@@ -8633,7 +8643,7 @@
         <v>231</v>
       </c>
       <c r="G209" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H209" s="1">
         <v>45244</v>
@@ -8641,16 +8651,16 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="B210" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C210" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="D210" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="E210" t="s">
         <v>11</v>
@@ -8659,7 +8669,7 @@
         <v>232</v>
       </c>
       <c r="G210" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H210" s="1">
         <v>44408</v>
@@ -8667,16 +8677,16 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B211" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="C211" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="D211" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="E211" t="s">
         <v>47</v>
@@ -8685,7 +8695,7 @@
         <v>233</v>
       </c>
       <c r="G211" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H211" s="1">
         <v>45294</v>
@@ -8693,16 +8703,16 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B212" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="C212" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D212" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="E212" t="s">
         <v>11</v>
@@ -8711,7 +8721,7 @@
         <v>234</v>
       </c>
       <c r="G212" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H212" s="1">
         <v>45225</v>
@@ -8719,16 +8729,16 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="B213" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="C213" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="D213" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="E213" t="s">
         <v>23</v>
@@ -8737,7 +8747,7 @@
         <v>235</v>
       </c>
       <c r="G213" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H213" s="1">
         <v>45294</v>
@@ -8745,13 +8755,13 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B214" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="C214" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="D214" t="s">
         <v>26</v>
@@ -8763,7 +8773,7 @@
         <v>236</v>
       </c>
       <c r="G214" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H214" s="1">
         <v>44292</v>
@@ -8771,16 +8781,16 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="B215" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="C215" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="D215" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="E215" t="s">
         <v>11</v>
@@ -8789,7 +8799,7 @@
         <v>237</v>
       </c>
       <c r="G215" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H215" s="1">
         <v>45223</v>
@@ -8797,16 +8807,16 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="B216" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="C216" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="D216" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="E216" t="s">
         <v>47</v>
@@ -8815,7 +8825,7 @@
         <v>238</v>
       </c>
       <c r="G216" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H216" s="1">
         <v>44392</v>
@@ -8823,16 +8833,16 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="B217" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="C217" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="D217" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E217" t="s">
         <v>47</v>
@@ -8841,7 +8851,7 @@
         <v>239</v>
       </c>
       <c r="G217" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H217" s="1">
         <v>44392</v>
@@ -8849,16 +8859,16 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="B218" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="C218" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="D218" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="E218" t="s">
         <v>47</v>
@@ -8867,7 +8877,7 @@
         <v>240</v>
       </c>
       <c r="G218" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H218" s="1">
         <v>44519</v>
@@ -8875,16 +8885,16 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="B219" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="C219" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="D219" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E219" t="s">
         <v>47</v>
@@ -8893,7 +8903,7 @@
         <v>241</v>
       </c>
       <c r="G219" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H219" s="1">
         <v>45294</v>
@@ -8901,16 +8911,16 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="B220" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="C220" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="D220" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E220" t="s">
         <v>47</v>
@@ -8919,7 +8929,7 @@
         <v>242</v>
       </c>
       <c r="G220" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H220" s="1">
         <v>44392</v>
@@ -8927,16 +8937,16 @@
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="B221" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="C221" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="D221" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E221" t="s">
         <v>47</v>
@@ -8945,7 +8955,7 @@
         <v>243</v>
       </c>
       <c r="G221" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H221" s="1">
         <v>44392</v>
@@ -8953,16 +8963,16 @@
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B222" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="C222" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="D222" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="E222" t="s">
         <v>47</v>
@@ -8971,7 +8981,7 @@
         <v>244</v>
       </c>
       <c r="G222" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H222" s="1">
         <v>44911</v>
@@ -8979,16 +8989,16 @@
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="B223" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="C223" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="D223" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E223" t="s">
         <v>47</v>
@@ -8997,7 +9007,7 @@
         <v>245</v>
       </c>
       <c r="G223" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H223" s="1">
         <v>44426</v>
@@ -9005,16 +9015,16 @@
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="B224" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="C224" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="D224" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E224" t="s">
         <v>47</v>
@@ -9023,7 +9033,7 @@
         <v>246</v>
       </c>
       <c r="G224" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H224" s="1">
         <v>45294</v>
@@ -9031,16 +9041,16 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="B225" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="C225" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="D225" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="E225" t="s">
         <v>47</v>
@@ -9049,7 +9059,7 @@
         <v>247</v>
       </c>
       <c r="G225" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H225" s="1">
         <v>44392</v>
@@ -9057,16 +9067,16 @@
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="B226" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="C226" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="D226" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="E226" t="s">
         <v>47</v>
@@ -9075,7 +9085,7 @@
         <v>248</v>
       </c>
       <c r="G226" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H226" s="1">
         <v>44880</v>
@@ -9083,16 +9093,16 @@
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="B227" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="C227" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="D227" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="E227" t="s">
         <v>47</v>
@@ -9101,7 +9111,7 @@
         <v>249</v>
       </c>
       <c r="G227" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H227" s="1">
         <v>44880</v>
@@ -9109,13 +9119,13 @@
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="B228" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="C228" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="D228" t="s">
         <v>26</v>
@@ -9127,7 +9137,7 @@
         <v>250</v>
       </c>
       <c r="G228" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H228" s="1">
         <v>44426</v>
@@ -9135,13 +9145,13 @@
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="B229" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="C229" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
       <c r="D229" t="s">
         <v>26</v>
@@ -9153,7 +9163,7 @@
         <v>251</v>
       </c>
       <c r="G229" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H229" s="1">
         <v>44994</v>
@@ -9161,16 +9171,16 @@
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="B230" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="C230" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="D230" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="E230" t="s">
         <v>11</v>
@@ -9179,7 +9189,7 @@
         <v>252</v>
       </c>
       <c r="G230" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H230" s="1">
         <v>45225</v>
@@ -9187,16 +9197,16 @@
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="B231" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="C231" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="D231" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="E231" t="s">
         <v>11</v>
@@ -9205,7 +9215,7 @@
         <v>253</v>
       </c>
       <c r="G231" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H231" s="1">
         <v>45232</v>
@@ -9213,16 +9223,16 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="B232" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="C232" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="D232" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="E232" t="s">
         <v>11</v>
@@ -9231,7 +9241,7 @@
         <v>254</v>
       </c>
       <c r="G232" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H232" s="1">
         <v>45224</v>
@@ -9239,16 +9249,16 @@
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="B233" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="C233" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="D233" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="E233" t="s">
         <v>23</v>
@@ -9257,7 +9267,7 @@
         <v>255</v>
       </c>
       <c r="G233" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H233" s="1">
         <v>44606</v>
@@ -9265,16 +9275,16 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="B234" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="C234" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="D234" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="E234" t="s">
         <v>11</v>
@@ -9283,7 +9293,7 @@
         <v>256</v>
       </c>
       <c r="G234" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H234" s="1">
         <v>45224</v>
@@ -9291,16 +9301,16 @@
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="B235" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="C235" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="D235" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="E235" t="s">
         <v>11</v>
@@ -9309,7 +9319,7 @@
         <v>257</v>
       </c>
       <c r="G235" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H235" s="1">
         <v>44636</v>
@@ -9317,16 +9327,16 @@
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="B236" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="C236" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="D236" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="E236" t="s">
         <v>23</v>
@@ -9335,7 +9345,7 @@
         <v>258</v>
       </c>
       <c r="G236" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H236" s="1">
         <v>44623</v>
@@ -9343,16 +9353,16 @@
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="B237" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="C237" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="D237" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="E237" t="s">
         <v>23</v>
@@ -9361,7 +9371,7 @@
         <v>259</v>
       </c>
       <c r="G237" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H237" s="1">
         <v>44624</v>
@@ -9369,16 +9379,16 @@
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="B238" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="C238" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="D238" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="E238" t="s">
         <v>59</v>
@@ -9387,7 +9397,7 @@
         <v>260</v>
       </c>
       <c r="G238" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H238" s="1">
         <v>44994</v>
@@ -9395,16 +9405,16 @@
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B239" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C239" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="D239" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="E239" t="s">
         <v>59</v>
@@ -9413,7 +9423,7 @@
         <v>261</v>
       </c>
       <c r="G239" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H239" s="1">
         <v>44994</v>
@@ -9421,16 +9431,16 @@
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="B240" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="C240" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="D240" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="E240" t="s">
         <v>47</v>
@@ -9439,7 +9449,7 @@
         <v>262</v>
       </c>
       <c r="G240" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H240" s="1">
         <v>44663</v>
@@ -9447,16 +9457,16 @@
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="B241" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="C241" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="D241" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E241" t="s">
         <v>47</v>
@@ -9465,7 +9475,7 @@
         <v>263</v>
       </c>
       <c r="G241" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H241" s="1">
         <v>44663</v>
@@ -9473,16 +9483,16 @@
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="B242" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="C242" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="D242" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E242" t="s">
         <v>47</v>
@@ -9491,7 +9501,7 @@
         <v>264</v>
       </c>
       <c r="G242" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H242" s="1">
         <v>44663</v>
@@ -9499,16 +9509,16 @@
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="B243" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="C243" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="D243" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E243" t="s">
         <v>47</v>
@@ -9517,7 +9527,7 @@
         <v>265</v>
       </c>
       <c r="G243" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H243" s="1">
         <v>44663</v>
@@ -9525,16 +9535,16 @@
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="B244" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="C244" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="D244" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E244" t="s">
         <v>47</v>
@@ -9543,7 +9553,7 @@
         <v>266</v>
       </c>
       <c r="G244" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H244" s="1">
         <v>44663</v>
@@ -9551,16 +9561,16 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="B245" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="C245" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="D245" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E245" t="s">
         <v>47</v>
@@ -9569,7 +9579,7 @@
         <v>267</v>
       </c>
       <c r="G245" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H245" s="1">
         <v>44663</v>
@@ -9577,16 +9587,16 @@
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="B246" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="C246" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="D246" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="E246" t="s">
         <v>11</v>
@@ -9595,7 +9605,7 @@
         <v>268</v>
       </c>
       <c r="G246" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H246" s="1">
         <v>45225</v>
@@ -9603,16 +9613,16 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="B247" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C247" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="D247" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="E247" t="s">
         <v>11</v>
@@ -9621,7 +9631,7 @@
         <v>269</v>
       </c>
       <c r="G247" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H247" s="1">
         <v>45226</v>
@@ -9629,16 +9639,16 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="B248" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="C248" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="D248" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="E248" t="s">
         <v>11</v>
@@ -9647,7 +9657,7 @@
         <v>270</v>
       </c>
       <c r="G248" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H248" s="1">
         <v>45225</v>
@@ -9655,16 +9665,16 @@
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="B249" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="C249" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="D249" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="E249" t="s">
         <v>11</v>
@@ -9673,7 +9683,7 @@
         <v>271</v>
       </c>
       <c r="G249" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H249" s="1">
         <v>45225</v>
@@ -9681,16 +9691,16 @@
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="B250" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="C250" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="D250" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="E250" t="s">
         <v>11</v>
@@ -9699,7 +9709,7 @@
         <v>272</v>
       </c>
       <c r="G250" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H250" s="1">
         <v>45225</v>
@@ -9707,16 +9717,16 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="B251" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="C251" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="D251" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="E251" t="s">
         <v>11</v>
@@ -9725,7 +9735,7 @@
         <v>273</v>
       </c>
       <c r="G251" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H251" s="1">
         <v>45225</v>
@@ -9733,16 +9743,16 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
       <c r="B252" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="C252" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="D252" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E252" t="s">
         <v>47</v>
@@ -9751,7 +9761,7 @@
         <v>274</v>
       </c>
       <c r="G252" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H252" s="1">
         <v>44882</v>
@@ -9759,16 +9769,16 @@
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="B253" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="C253" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="D253" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="E253" t="s">
         <v>47</v>
@@ -9777,7 +9787,7 @@
         <v>275</v>
       </c>
       <c r="G253" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H253" s="1">
         <v>44882</v>
@@ -9785,16 +9795,16 @@
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
+        <v>803</v>
+      </c>
+      <c r="B254" t="s">
         <v>809</v>
       </c>
-      <c r="B254" t="s">
-        <v>815</v>
-      </c>
       <c r="C254" t="s">
+        <v>804</v>
+      </c>
+      <c r="D254" t="s">
         <v>810</v>
-      </c>
-      <c r="D254" t="s">
-        <v>816</v>
       </c>
       <c r="E254" t="s">
         <v>47</v>
@@ -9803,7 +9813,7 @@
         <v>276</v>
       </c>
       <c r="G254" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H254" s="1">
         <v>44914</v>
@@ -9811,16 +9821,16 @@
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="B255" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="C255" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="D255" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="E255" t="s">
         <v>47</v>
@@ -9829,7 +9839,7 @@
         <v>277</v>
       </c>
       <c r="G255" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H255" s="1">
         <v>45294</v>
@@ -9837,16 +9847,16 @@
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="B256" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="C256" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="D256" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="E256" t="s">
         <v>23</v>
@@ -9855,7 +9865,7 @@
         <v>278</v>
       </c>
       <c r="G256" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H256" s="1">
         <v>44999</v>
@@ -9863,16 +9873,16 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="B257" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="C257" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="D257" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="E257" t="s">
         <v>23</v>
@@ -9881,7 +9891,7 @@
         <v>279</v>
       </c>
       <c r="G257" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H257" s="1">
         <v>45083</v>
@@ -9889,16 +9899,16 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B258" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="C258" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="D258" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="E258" t="s">
         <v>11</v>
@@ -9907,7 +9917,7 @@
         <v>280</v>
       </c>
       <c r="G258" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H258" s="1">
         <v>45294</v>
@@ -9915,16 +9925,16 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="B259" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="C259" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="D259" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="E259" t="s">
         <v>23</v>
@@ -9933,7 +9943,7 @@
         <v>281</v>
       </c>
       <c r="G259" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H259" s="1">
         <v>45120</v>
@@ -9941,16 +9951,16 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="B260" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="C260" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="D260" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="E260" t="s">
         <v>23</v>
@@ -9959,7 +9969,7 @@
         <v>282</v>
       </c>
       <c r="G260" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H260" s="1">
         <v>45132</v>
@@ -9967,16 +9977,16 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="B261" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="C261" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="D261" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="E261" t="s">
         <v>23</v>
@@ -9985,7 +9995,7 @@
         <v>283</v>
       </c>
       <c r="G261" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H261" s="1">
         <v>45147</v>
@@ -9993,16 +10003,16 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="B262" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="C262" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="D262" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="E262" t="s">
         <v>23</v>
@@ -10011,7 +10021,7 @@
         <v>284</v>
       </c>
       <c r="G262" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H262" s="1">
         <v>45170</v>
@@ -10019,16 +10029,16 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="B263" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="C263" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="D263" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="E263" t="s">
         <v>23</v>
@@ -10037,7 +10047,7 @@
         <v>285</v>
       </c>
       <c r="G263" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H263" s="1">
         <v>45182</v>
@@ -10045,16 +10055,16 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="B264" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="C264" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="D264" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="E264" t="s">
         <v>23</v>
@@ -10063,7 +10073,7 @@
         <v>286</v>
       </c>
       <c r="G264" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H264" s="1">
         <v>45182</v>
@@ -10071,16 +10081,16 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="B265" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="C265" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="D265" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="E265" t="s">
         <v>23</v>
@@ -10089,7 +10099,7 @@
         <v>287</v>
       </c>
       <c r="G265" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H265" s="1">
         <v>45182</v>
@@ -10097,16 +10107,16 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="B266" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="C266" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="D266" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="E266" t="s">
         <v>23</v>
@@ -10115,7 +10125,7 @@
         <v>288</v>
       </c>
       <c r="G266" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H266" s="1">
         <v>45182</v>
@@ -10123,16 +10133,16 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="B267" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="C267" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="D267" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="E267" t="s">
         <v>23</v>
@@ -10141,7 +10151,7 @@
         <v>289</v>
       </c>
       <c r="G267" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H267" s="1">
         <v>45182</v>
@@ -10149,16 +10159,16 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="B268" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="C268" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="D268" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="E268" t="s">
         <v>11</v>
@@ -10167,7 +10177,7 @@
         <v>290</v>
       </c>
       <c r="G268" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H268" s="1">
         <v>45188</v>
@@ -10175,16 +10185,16 @@
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="B269" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="C269" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="D269" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="E269" t="s">
         <v>11</v>
@@ -10193,7 +10203,7 @@
         <v>291</v>
       </c>
       <c r="G269" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H269" s="1">
         <v>45188</v>
@@ -10201,16 +10211,16 @@
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="B270" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="C270" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="D270" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="E270" t="s">
         <v>23</v>
@@ -10219,7 +10229,7 @@
         <v>292</v>
       </c>
       <c r="G270" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H270" s="1">
         <v>45316</v>
@@ -10227,16 +10237,16 @@
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="B271" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="C271" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="D271" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="E271" t="s">
         <v>23</v>
@@ -10245,7 +10255,7 @@
         <v>293</v>
       </c>
       <c r="G271" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H271" s="1">
         <v>45280</v>
@@ -10253,16 +10263,16 @@
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="B272" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="C272" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="D272" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="E272" t="s">
         <v>23</v>
@@ -10271,7 +10281,7 @@
         <v>294</v>
       </c>
       <c r="G272" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H272" s="1">
         <v>45316</v>
@@ -10279,16 +10289,16 @@
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>795</v>
+        <v>923</v>
       </c>
       <c r="B273" t="s">
-        <v>796</v>
+        <v>924</v>
       </c>
       <c r="C273" t="s">
-        <v>797</v>
+        <v>924</v>
       </c>
       <c r="D273" t="s">
-        <v>898</v>
+        <v>925</v>
       </c>
       <c r="E273" t="s">
         <v>11</v>
@@ -10297,9 +10307,35 @@
         <v>295</v>
       </c>
       <c r="G273" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H273" s="1">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>789</v>
+      </c>
+      <c r="B274" t="s">
+        <v>790</v>
+      </c>
+      <c r="C274" t="s">
+        <v>791</v>
+      </c>
+      <c r="D274" t="s">
+        <v>892</v>
+      </c>
+      <c r="E274" t="s">
+        <v>11</v>
+      </c>
+      <c r="F274">
+        <v>296</v>
+      </c>
+      <c r="G274" t="s">
+        <v>600</v>
+      </c>
+      <c r="H274" s="1">
         <v>45225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update codesets and versions and setup Dockerfile and build script
</commit_message>
<xml_diff>
--- a/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
+++ b/cds-tcamt/cds-tcamt-controller/src/main/resources/codeset/web_cvx.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/ske5_cdc_gov/Documents/+My_Documents/Shilpa/CPT/downloads/New/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="658" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{799BB4FB-62B2-4662-A90E-A9490E63CE75}"/>
+  <xr:revisionPtr revIDLastSave="681" documentId="13_ncr:1_{4E4CFCED-0B0A-43B8-A237-65405DFDA4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7FD9DD2-A25C-49E8-A270-53994C64AC3C}"/>
   <bookViews>
-    <workbookView xWindow="1788" yWindow="936" windowWidth="21252" windowHeight="10932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Web_cvx" sheetId="71" r:id="rId1"/>
+    <sheet name="Web_cvx" sheetId="72" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" localSheetId="0" hidden="1">Web_cvx!$A$1:$H$280</definedName>
+    <definedName name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" localSheetId="0" hidden="1">Web_cvx!$A$1:$H$281</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -24,14 +24,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{F122FED2-8D7A-4D71-8572-501271B3B1D2}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes11111111111111111111111111111111111111111111111111" type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{6E74380E-EF49-4442-9B15-CEA084F22A8F}" odcFile="\\cdc.gov\private\M314\ske5\My Data Sources\DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes.odc" keepAlive="1" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes111111111111111111111111111111111111111111111111111" type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;User ID=insidenipdbo;Initial Catalog=NIP_INSIDENIP;Data Source=DSDV-INFC-1601\qsrv1;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=D314248;Use Encryption for Data=False;Tag with column collation when possible=False" command="&quot;NIP_INSIDENIP&quot;.&quot;dbo&quot;.&quot;tblCVXCodes&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="948">
   <si>
     <t>CVX Code</t>
   </si>
@@ -2862,10 +2862,19 @@
     <t xml:space="preserve">Unspecified code H5xx vaccines to be used when specific formulation is unknown - for vaccines administered starting 2024 </t>
   </si>
   <si>
-    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ, (nirsevimab-alip), 0.5 mL, neonates and children to 24 months</t>
-  </si>
-  <si>
-    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ, (nirsevimab-alip), 1 mL, neonates and children to 24 months</t>
+    <t>327</t>
+  </si>
+  <si>
+    <t>Pneumococcal conjugate PCV21, polysaccharide CRM197 conjugate, PF</t>
+  </si>
+  <si>
+    <t>Pneumococcal conjugate vaccine, 21 valent (PCV21), polysaccharide CRM197 conjugate, preservative free</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ , (nirsevimab-alip), 0.5 mL, neonates and children to 24 months</t>
+  </si>
+  <si>
+    <t>Respiratory syncytial virus (RSV) monoclonal antibody, IgG1κ , (nirsevimab-alip), 1 mL, neonates and children to 24 months</t>
   </si>
 </sst>
 </file>
@@ -2929,7 +2938,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" connectionId="1" xr16:uid="{1E523728-59BB-4929-BE00-655637F4CA7B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DSDV-INFC-1601_qsrv1 NIP_INSIDENIP tblCVXCodes" connectionId="1" xr16:uid="{820F95D8-8905-4A7F-B770-D3800C2AA8D5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="11">
     <queryTableFields count="8">
       <queryTableField id="2" name="cvx_code" tableColumnId="2"/>
@@ -2949,16 +2958,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1434D6D-708D-4380-9421-3840925443E0}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes_1" ref="A1:H280" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8584E41-B2DB-4C7C-BCE9-42832A4AD29E}" name="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" displayName="Table_DSDV_INFC_1601_qsrv1_NIP_INSIDENIP_tblCVXCodes" ref="A1:H281" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{425F6119-1CAC-481D-974B-9A53D5370240}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{66BF3BCC-4A62-4524-827B-867C99DEE14A}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{184C084A-5955-4026-8114-FA5BF1BFA269}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{26405ED7-245E-49FE-8861-6348A80FE43A}" uniqueName="5" name="Note" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{7D9F5ECD-8721-4B27-B9AB-EB25EE327C3C}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
-    <tableColumn id="1" xr3:uid="{F4D15D66-BCA4-4D30-B80F-3B54843374E4}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
-    <tableColumn id="8" xr3:uid="{0FDA1B71-36AD-42F3-9A41-C3D8D3258F45}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{8FE42A1E-FF55-409A-A3FE-7B78A8D55D6A}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5547DD2F-73B5-41CB-ABE0-D016542BC608}" uniqueName="2" name="CVX Code" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{1F5DB54C-D489-4BBF-8611-26399EF7EE03}" uniqueName="3" name="CVX Short Description" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{838FD752-E6A0-4D44-BC1E-2513C50F7F36}" uniqueName="4" name="Full Vaccine Name" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{AE06D11E-34CC-4778-B41B-B6AD7106870D}" uniqueName="5" name="Note" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{28DB2BAA-3376-45DF-8EA1-88FA0D5C59B3}" uniqueName="6" name="VaccineStatus" queryTableFieldId="6"/>
+    <tableColumn id="1" xr3:uid="{016014BD-5688-4F22-A266-DEAD493F9A39}" uniqueName="1" name="internalID" queryTableFieldId="1"/>
+    <tableColumn id="8" xr3:uid="{624389A5-8306-4A55-95F7-758EC4658A0D}" uniqueName="8" name="nonvaccine" queryTableFieldId="8"/>
+    <tableColumn id="9" xr3:uid="{C4ECF28B-E430-4850-B6D7-A7BD5E367EE2}" uniqueName="9" name="update_date" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3250,24 +3259,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D97E6F-DF47-4B82-AB2F-3D53C3DBE81D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A7C482-A330-4CBB-B47E-F284871B8414}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H280"/>
+  <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="C254" sqref="C254"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7532,7 +7541,7 @@
         <v>571</v>
       </c>
       <c r="H164" s="1">
-        <v>41843</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
@@ -9799,19 +9808,19 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
       <c r="B252" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="C252" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="D252" t="s">
-        <v>652</v>
+        <v>857</v>
       </c>
       <c r="E252" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F252">
         <v>274</v>
@@ -9820,7 +9829,7 @@
         <v>571</v>
       </c>
       <c r="H252" s="1">
-        <v>44882</v>
+        <v>45225</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.3">
@@ -10013,7 +10022,7 @@
         <v>809</v>
       </c>
       <c r="C260" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
       <c r="D260" t="s">
         <v>810</v>
@@ -10039,7 +10048,7 @@
         <v>812</v>
       </c>
       <c r="C261" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="D261" t="s">
         <v>810</v>
@@ -10475,19 +10484,19 @@
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="B278" t="s">
-        <v>758</v>
+        <v>765</v>
       </c>
       <c r="C278" t="s">
-        <v>759</v>
+        <v>766</v>
       </c>
       <c r="D278" t="s">
-        <v>857</v>
+        <v>652</v>
       </c>
       <c r="E278" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="F278">
         <v>300</v>
@@ -10496,7 +10505,7 @@
         <v>571</v>
       </c>
       <c r="H278" s="1">
-        <v>45225</v>
+        <v>44882</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.3">
@@ -10527,19 +10536,19 @@
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="B280" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="C280" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c r="D280" t="s">
-        <v>942</v>
+        <v>26</v>
       </c>
       <c r="E280" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F280">
         <v>302</v>
@@ -10548,6 +10557,32 @@
         <v>571</v>
       </c>
       <c r="H280" s="1">
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>940</v>
+      </c>
+      <c r="B281" t="s">
+        <v>941</v>
+      </c>
+      <c r="C281" t="s">
+        <v>941</v>
+      </c>
+      <c r="D281" t="s">
+        <v>942</v>
+      </c>
+      <c r="E281" t="s">
+        <v>11</v>
+      </c>
+      <c r="F281">
+        <v>303</v>
+      </c>
+      <c r="G281" t="s">
+        <v>571</v>
+      </c>
+      <c r="H281" s="1">
         <v>45449</v>
       </c>
     </row>

</xml_diff>